<commit_message>
01: Working on experimental part
</commit_message>
<xml_diff>
--- a/01_Townsend/data/Townsend.xlsx
+++ b/01_Townsend/data/Townsend.xlsx
@@ -1,17 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\Škola Mgr\Praktikum plazma\PraktikaPlazma\01_Townsend\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D6EC54-A580-498D-931D-814A39F82F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="9555" windowHeight="8010"/>
+    <workbookView xWindow="15735" yWindow="3375" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -120,7 +138,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -171,7 +189,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -179,12 +197,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -226,7 +247,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -259,9 +280,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -294,6 +332,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -469,11 +524,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2665,7 +2720,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2677,7 +2732,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
01: Progress in experimental part
</commit_message>
<xml_diff>
--- a/01_Townsend/data/Townsend.xlsx
+++ b/01_Townsend/data/Townsend.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\Škola Mgr\Praktikum plazma\PraktikaPlazma\01_Townsend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D6EC54-A580-498D-931D-814A39F82F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7139579-E3F6-48FD-9967-2F0CCF252600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15735" yWindow="3375" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6000" yWindow="2850" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="34">
   <si>
     <t>Vcm-1</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>alpha [m-1]</t>
+  </si>
+  <si>
+    <t>exp fit</t>
   </si>
 </sst>
 </file>
@@ -525,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T64"/>
+  <dimension ref="A1:Z64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,9 +539,11 @@
     <col min="10" max="11" width="9.140625" style="3"/>
     <col min="12" max="12" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
@@ -559,7 +564,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -600,7 +605,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>85</f>
         <v>85</v>
@@ -640,7 +645,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+2</f>
         <v>87</v>
@@ -680,7 +685,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:A12" si="3">A4+2</f>
         <v>89</v>
@@ -720,7 +725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="3"/>
         <v>91</v>
@@ -760,7 +765,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="3"/>
         <v>93</v>
@@ -800,7 +805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="3"/>
         <v>95</v>
@@ -837,7 +842,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="3"/>
         <v>97</v>
@@ -873,8 +878,11 @@
       <c r="L9" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="3"/>
         <v>99</v>
@@ -928,8 +936,26 @@
       <c r="R10" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="W10" t="s">
+        <v>19</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="3"/>
         <v>101</v>
@@ -975,8 +1001,17 @@
         <f>EXP(N11)</f>
         <v>44.647575243891616</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T11" s="3">
+        <v>80</v>
+      </c>
+      <c r="U11">
+        <v>1.6020799999999999</v>
+      </c>
+      <c r="Y11">
+        <v>63.650860000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="3"/>
         <v>103</v>
@@ -1022,8 +1057,17 @@
         <f t="shared" ref="Q12:Q20" si="5">EXP(N12)</f>
         <v>1.0554846021550801</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="U12">
+        <v>5.722E-2</v>
+      </c>
+      <c r="Y12">
+        <v>6.6234200000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L13" s="3">
         <v>90</v>
       </c>
@@ -1037,8 +1081,17 @@
         <f t="shared" si="5"/>
         <v>30.153771302174523</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T13" s="3">
+        <v>90</v>
+      </c>
+      <c r="U13">
+        <v>1.8524799999999999</v>
+      </c>
+      <c r="Y13">
+        <v>45.298009999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1061,8 +1114,17 @@
         <f t="shared" si="5"/>
         <v>1.1102664149565653</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="U14">
+        <v>3.3259999999999998E-2</v>
+      </c>
+      <c r="Y14">
+        <v>2.79297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1091,8 +1153,17 @@
         <f t="shared" si="5"/>
         <v>15.315723799642379</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T15" s="3">
+        <v>100</v>
+      </c>
+      <c r="U15">
+        <v>2.0671499999999998</v>
+      </c>
+      <c r="Y15">
+        <v>26.650030000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>85</f>
         <v>85</v>
@@ -1138,8 +1209,17 @@
         <f t="shared" si="5"/>
         <v>1.1165236786502826</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="U16">
+        <v>3.3950000000000001E-2</v>
+      </c>
+      <c r="Y16">
+        <v>1.6993199999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>A16+2</f>
         <v>87</v>
@@ -1185,8 +1265,17 @@
         <f t="shared" si="5"/>
         <v>12.249192298492478</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T17" s="3">
+        <v>110</v>
+      </c>
+      <c r="U17">
+        <v>2.2840400000000001</v>
+      </c>
+      <c r="Y17">
+        <v>19.918209999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ref="A18:A25" si="9">A17+2</f>
         <v>89</v>
@@ -1232,8 +1321,17 @@
         <f t="shared" si="5"/>
         <v>1.1160436766762836</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="U18">
+        <v>3.2439999999999997E-2</v>
+      </c>
+      <c r="Y18">
+        <v>1.22679</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="9"/>
         <v>91</v>
@@ -1279,8 +1377,17 @@
         <f t="shared" si="5"/>
         <v>3.7323945567549304</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T19" s="3">
+        <v>120</v>
+      </c>
+      <c r="U19">
+        <v>2.7830599999999999</v>
+      </c>
+      <c r="Y19">
+        <v>7.0880000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="9"/>
         <v>93</v>
@@ -1326,8 +1433,17 @@
         <f t="shared" si="5"/>
         <v>1.2846418968311495</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="U20">
+        <v>3.5029999999999999E-2</v>
+      </c>
+      <c r="Y20">
+        <v>0.48057</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="9"/>
         <v>95</v>
@@ -1360,8 +1476,9 @@
         <f t="shared" si="4"/>
         <v>5.706002231394514</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T21" s="3"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="9"/>
         <v>97</v>
@@ -1409,8 +1526,23 @@
       <c r="P22" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="V22" t="s">
+        <v>28</v>
+      </c>
+      <c r="W22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="X22" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="9"/>
         <v>99</v>
@@ -1462,8 +1594,27 @@
         <f>$L$1/L23</f>
         <v>9.9375000000000002E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T23" s="3">
+        <v>8000</v>
+      </c>
+      <c r="U23">
+        <f>U11*100</f>
+        <v>160.208</v>
+      </c>
+      <c r="V23">
+        <f>U23/$L$1</f>
+        <v>2.0151949685534589</v>
+      </c>
+      <c r="W23">
+        <f>LN(V23)</f>
+        <v>0.70071594930516068</v>
+      </c>
+      <c r="X23">
+        <f>$L$1/T23</f>
+        <v>9.9375000000000002E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="9"/>
         <v>101</v>
@@ -1515,8 +1666,27 @@
         <f t="shared" ref="P24:P27" si="12">$L$1/L24</f>
         <v>8.8333333333333337E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T24" s="3">
+        <v>9000</v>
+      </c>
+      <c r="U24">
+        <f>U13*100</f>
+        <v>185.24799999999999</v>
+      </c>
+      <c r="V24">
+        <f t="shared" ref="V24:V27" si="13">U24/$L$1</f>
+        <v>2.3301635220125787</v>
+      </c>
+      <c r="W24">
+        <f t="shared" ref="W24:W27" si="14">LN(V24)</f>
+        <v>0.84593844623630798</v>
+      </c>
+      <c r="X24">
+        <f t="shared" ref="X24:X27" si="15">$L$1/T24</f>
+        <v>8.8333333333333337E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="9"/>
         <v>103</v>
@@ -1568,8 +1738,27 @@
         <f t="shared" si="12"/>
         <v>7.9500000000000005E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T25" s="3">
+        <v>10000</v>
+      </c>
+      <c r="U25">
+        <f>U15*100</f>
+        <v>206.71499999999997</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="13"/>
+        <v>2.6001886792452829</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="14"/>
+        <v>0.95558401133493154</v>
+      </c>
+      <c r="X25">
+        <f t="shared" si="15"/>
+        <v>7.9500000000000005E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="L26" s="3">
         <v>11000</v>
       </c>
@@ -1589,8 +1778,27 @@
         <f t="shared" si="12"/>
         <v>7.2272727272727271E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T26" s="3">
+        <v>11000</v>
+      </c>
+      <c r="U26">
+        <f>U17*100</f>
+        <v>228.404</v>
+      </c>
+      <c r="V26">
+        <f>U26/$L$1</f>
+        <v>2.8730062893081763</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="14"/>
+        <v>1.0553589691030669</v>
+      </c>
+      <c r="X26">
+        <f t="shared" si="15"/>
+        <v>7.2272727272727271E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>0</v>
       </c>
@@ -1619,8 +1827,27 @@
         <f t="shared" si="12"/>
         <v>6.6249999999999998E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T27" s="3">
+        <v>12000</v>
+      </c>
+      <c r="U27">
+        <f>U19*100</f>
+        <v>278.30599999999998</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="13"/>
+        <v>3.5007044025157232</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="14"/>
+        <v>1.2529642061073567</v>
+      </c>
+      <c r="X27">
+        <f t="shared" si="15"/>
+        <v>6.6249999999999998E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1637,7 +1864,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>85</f>
         <v>85</v>
@@ -1650,7 +1877,7 @@
         <v>180</v>
       </c>
       <c r="D29">
-        <f t="shared" ref="D29:D38" si="13">C29/2</f>
+        <f t="shared" ref="D29:D38" si="16">C29/2</f>
         <v>90</v>
       </c>
       <c r="E29" s="2">
@@ -1671,7 +1898,7 @@
         <v>7.5186072168152522</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>A29+2</f>
         <v>87</v>
@@ -1680,15 +1907,15 @@
         <v>1.8</v>
       </c>
       <c r="C30">
-        <f t="shared" ref="C30:C38" si="14">C$27*$B30</f>
+        <f t="shared" ref="C30:C38" si="17">C$27*$B30</f>
         <v>162</v>
       </c>
       <c r="D30">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>81</v>
       </c>
       <c r="E30" s="2">
-        <f t="shared" ref="E30:E38" si="15">AVERAGE(F30,G30,H30)</f>
+        <f t="shared" ref="E30:E38" si="18">AVERAGE(F30,G30,H30)</f>
         <v>1247.6666666666667</v>
       </c>
       <c r="F30">
@@ -1701,28 +1928,28 @@
         <v>1235</v>
       </c>
       <c r="J30" s="3">
-        <f t="shared" ref="J30:J64" si="16">LN(E30)</f>
+        <f t="shared" ref="J30:J64" si="19">LN(E30)</f>
         <v>7.1290304192363196</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" ref="A31:A38" si="17">A30+2</f>
+        <f t="shared" ref="A31:A38" si="20">A30+2</f>
         <v>89</v>
       </c>
       <c r="B31" s="1">
         <v>1.6</v>
       </c>
       <c r="C31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>144</v>
       </c>
       <c r="D31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>72</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>898.66666666666663</v>
       </c>
       <c r="F31">
@@ -1735,28 +1962,28 @@
         <v>901</v>
       </c>
       <c r="J31" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>6.8009121833640878</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>91</v>
       </c>
       <c r="B32" s="1">
         <v>1.4</v>
       </c>
       <c r="C32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>125.99999999999999</v>
       </c>
       <c r="D32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>62.999999999999993</v>
       </c>
       <c r="E32" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>629.33333333333337</v>
       </c>
       <c r="F32">
@@ -1769,28 +1996,28 @@
         <v>635</v>
       </c>
       <c r="J32" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>6.4446610580373367</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>93</v>
       </c>
       <c r="B33" s="1">
         <v>1.2</v>
       </c>
       <c r="C33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>108</v>
       </c>
       <c r="D33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>54</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>437</v>
       </c>
       <c r="F33">
@@ -1803,28 +2030,28 @@
         <v>444</v>
       </c>
       <c r="J33" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>6.0799331950955899</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>95</v>
       </c>
       <c r="B34" s="1">
         <v>1</v>
       </c>
       <c r="C34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>90</v>
       </c>
       <c r="D34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>45</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>278.66666666666669</v>
       </c>
       <c r="F34">
@@ -1837,28 +2064,28 @@
         <v>276</v>
       </c>
       <c r="J34" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>5.6300163244165917</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>97</v>
       </c>
       <c r="B35" s="1">
         <v>0.8</v>
       </c>
       <c r="C35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>72</v>
       </c>
       <c r="D35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>36</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>187.66666666666666</v>
       </c>
       <c r="F35">
@@ -1871,28 +2098,28 @@
         <v>188</v>
       </c>
       <c r="J35" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>5.2346673394715806</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>99</v>
       </c>
       <c r="B36" s="1">
         <v>0.6</v>
       </c>
       <c r="C36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>54</v>
       </c>
       <c r="D36">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>27</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>121</v>
       </c>
       <c r="F36">
@@ -1905,28 +2132,28 @@
         <v>119</v>
       </c>
       <c r="J36" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>4.7957905455967413</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>101</v>
       </c>
       <c r="B37" s="1">
         <v>0.4</v>
       </c>
       <c r="C37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>36</v>
       </c>
       <c r="D37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>18</v>
       </c>
       <c r="E37" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>72</v>
       </c>
       <c r="F37">
@@ -1939,28 +2166,28 @@
         <v>72</v>
       </c>
       <c r="J37" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>4.2766661190160553</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>103</v>
       </c>
       <c r="B38" s="1">
         <v>0.2</v>
       </c>
       <c r="C38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>18</v>
       </c>
       <c r="D38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>9</v>
       </c>
       <c r="E38" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>33.666666666666664</v>
       </c>
       <c r="F38">
@@ -1973,7 +2200,7 @@
         <v>32</v>
       </c>
       <c r="J38" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>3.5165082281731497</v>
       </c>
     </row>
@@ -2018,7 +2245,7 @@
         <v>220</v>
       </c>
       <c r="D42">
-        <f t="shared" ref="D42:D51" si="18">C42/2</f>
+        <f t="shared" ref="D42:D51" si="21">C42/2</f>
         <v>110</v>
       </c>
       <c r="E42" s="2">
@@ -2035,7 +2262,7 @@
         <v>1895</v>
       </c>
       <c r="J42" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>7.5504859736280663</v>
       </c>
     </row>
@@ -2048,15 +2275,15 @@
         <v>1.8</v>
       </c>
       <c r="C43">
-        <f t="shared" ref="C43:C51" si="19">C$40*$B43</f>
+        <f t="shared" ref="C43:C51" si="22">C$40*$B43</f>
         <v>198</v>
       </c>
       <c r="D43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>99</v>
       </c>
       <c r="E43" s="2">
-        <f t="shared" ref="E43:E51" si="20">AVERAGE(F43,G43,H43)</f>
+        <f t="shared" ref="E43:E51" si="23">AVERAGE(F43,G43,H43)</f>
         <v>1243.6666666666667</v>
       </c>
       <c r="F43">
@@ -2069,28 +2296,28 @@
         <v>1241</v>
       </c>
       <c r="J43" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>7.1258192845530486</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" ref="A44:A51" si="21">A43+2</f>
+        <f t="shared" ref="A44:A51" si="24">A43+2</f>
         <v>89</v>
       </c>
       <c r="B44" s="1">
         <v>1.6</v>
       </c>
       <c r="C44">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>176</v>
       </c>
       <c r="D44">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>88</v>
       </c>
       <c r="E44" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>785.66666666666663</v>
       </c>
       <c r="F44">
@@ -2103,28 +2330,28 @@
         <v>789</v>
       </c>
       <c r="J44" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>6.6665326142680215</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>91</v>
       </c>
       <c r="B45" s="1">
         <v>1.4</v>
       </c>
       <c r="C45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>154</v>
       </c>
       <c r="D45">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>77</v>
       </c>
       <c r="E45" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>478</v>
       </c>
       <c r="F45">
@@ -2137,28 +2364,28 @@
         <v>477</v>
       </c>
       <c r="J45" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>6.1696107324914564</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>93</v>
       </c>
       <c r="B46" s="1">
         <v>1.2</v>
       </c>
       <c r="C46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>132</v>
       </c>
       <c r="D46">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>66</v>
       </c>
       <c r="E46" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>302</v>
       </c>
       <c r="F46">
@@ -2171,28 +2398,28 @@
         <v>297</v>
       </c>
       <c r="J46" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>5.7104270173748697</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>95</v>
       </c>
       <c r="B47" s="1">
         <v>1</v>
       </c>
       <c r="C47">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>110</v>
       </c>
       <c r="D47">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>55</v>
       </c>
       <c r="E47" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>181</v>
       </c>
       <c r="F47">
@@ -2205,28 +2432,28 @@
         <v>185</v>
       </c>
       <c r="J47" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>5.1984970312658261</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>97</v>
       </c>
       <c r="B48" s="1">
         <v>0.8</v>
       </c>
       <c r="C48">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>88</v>
       </c>
       <c r="D48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>44</v>
       </c>
       <c r="E48" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>116</v>
       </c>
       <c r="F48">
@@ -2239,28 +2466,28 @@
         <v>112</v>
       </c>
       <c r="J48" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>4.7535901911063645</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>99</v>
       </c>
       <c r="B49" s="1">
         <v>0.6</v>
       </c>
       <c r="C49">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>66</v>
       </c>
       <c r="D49">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>33</v>
       </c>
       <c r="E49" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>66.666666666666671</v>
       </c>
       <c r="F49">
@@ -2273,28 +2500,28 @@
         <v>65</v>
       </c>
       <c r="J49" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>4.1997050778799272</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>101</v>
       </c>
       <c r="B50" s="1">
         <v>0.4</v>
       </c>
       <c r="C50">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>44</v>
       </c>
       <c r="D50">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>22</v>
       </c>
       <c r="E50" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>35.666666666666664</v>
       </c>
       <c r="F50">
@@ -2307,28 +2534,28 @@
         <v>38</v>
       </c>
       <c r="J50" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>3.5742165457937962</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>103</v>
       </c>
       <c r="B51" s="1">
         <v>0.2</v>
       </c>
       <c r="C51">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>22</v>
       </c>
       <c r="D51">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
       <c r="E51" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>14.666666666666666</v>
       </c>
       <c r="F51">
@@ -2341,7 +2568,7 @@
         <v>15</v>
       </c>
       <c r="J51" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>2.6855773452501515</v>
       </c>
     </row>
@@ -2386,11 +2613,11 @@
         <v>240</v>
       </c>
       <c r="D55">
-        <f t="shared" ref="D55:D64" si="22">C55/2</f>
+        <f t="shared" ref="D55:D64" si="25">C55/2</f>
         <v>120</v>
       </c>
       <c r="E55" s="2">
-        <f t="shared" ref="E55:E64" si="23">AVERAGE(F55,G55,H55)</f>
+        <f t="shared" ref="E55:E64" si="26">AVERAGE(F55,G55,H55)</f>
         <v>1862.3333333333333</v>
       </c>
       <c r="F55">
@@ -2403,7 +2630,7 @@
         <v>1858</v>
       </c>
       <c r="J55" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>7.5295854607910391</v>
       </c>
     </row>
@@ -2416,15 +2643,15 @@
         <v>1.8</v>
       </c>
       <c r="C56">
-        <f t="shared" ref="C56:C64" si="24">C$53*$B56</f>
+        <f t="shared" ref="C56:C64" si="27">C$53*$B56</f>
         <v>216</v>
       </c>
       <c r="D56">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>108</v>
       </c>
       <c r="E56" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>1043.6666666666667</v>
       </c>
       <c r="F56">
@@ -2437,28 +2664,28 @@
         <v>1045</v>
       </c>
       <c r="J56" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>6.9504954326582959</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" ref="A57:A64" si="25">A56+2</f>
+        <f t="shared" ref="A57:A64" si="28">A56+2</f>
         <v>89</v>
       </c>
       <c r="B57" s="1">
         <v>1.6</v>
       </c>
       <c r="C57">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>192</v>
       </c>
       <c r="D57">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>96</v>
       </c>
       <c r="E57" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>598.66666666666663</v>
       </c>
       <c r="F57">
@@ -2471,28 +2698,28 @@
         <v>600</v>
       </c>
       <c r="J57" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>6.3947049601940353</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>91</v>
       </c>
       <c r="B58" s="1">
         <v>1.4</v>
       </c>
       <c r="C58">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>168</v>
       </c>
       <c r="D58">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>84</v>
       </c>
       <c r="E58" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>353.66666666666669</v>
       </c>
       <c r="F58">
@@ -2505,28 +2732,28 @@
         <v>352</v>
       </c>
       <c r="J58" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>5.8683548499458738</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>93</v>
       </c>
       <c r="B59" s="1">
         <v>1.2</v>
       </c>
       <c r="C59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>144</v>
       </c>
       <c r="D59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>72</v>
       </c>
       <c r="E59" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>224.66666666666666</v>
       </c>
       <c r="F59">
@@ -2539,28 +2766,28 @@
         <v>223</v>
       </c>
       <c r="J59" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>5.414617822244197</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>95</v>
       </c>
       <c r="B60" s="1">
         <v>1</v>
       </c>
       <c r="C60">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>120</v>
       </c>
       <c r="D60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>60</v>
       </c>
       <c r="E60" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>125</v>
       </c>
       <c r="F60">
@@ -2573,28 +2800,28 @@
         <v>122</v>
       </c>
       <c r="J60" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>4.8283137373023015</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>97</v>
       </c>
       <c r="B61" s="1">
         <v>0.8</v>
       </c>
       <c r="C61">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>96</v>
       </c>
       <c r="D61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>48</v>
       </c>
       <c r="E61" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>76.333333333333329</v>
       </c>
       <c r="F61">
@@ -2607,28 +2834,28 @@
         <v>82</v>
       </c>
       <c r="J61" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>4.33510971488613</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>99</v>
       </c>
       <c r="B62" s="1">
         <v>0.6</v>
       </c>
       <c r="C62">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>72</v>
       </c>
       <c r="D62">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>36</v>
       </c>
       <c r="E62" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>34.333333333333336</v>
       </c>
       <c r="F62">
@@ -2641,28 +2868,28 @@
         <v>34</v>
       </c>
       <c r="J62" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>3.5361166995615263</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>101</v>
       </c>
       <c r="B63" s="1">
         <v>0.4</v>
       </c>
       <c r="C63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>48</v>
       </c>
       <c r="D63">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>24</v>
       </c>
       <c r="E63" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>14</v>
       </c>
       <c r="F63">
@@ -2675,28 +2902,28 @@
         <v>16</v>
       </c>
       <c r="J63" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>2.6390573296152584</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>103</v>
       </c>
       <c r="B64" s="1">
         <v>0.2</v>
       </c>
       <c r="C64">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>24</v>
       </c>
       <c r="D64">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>12</v>
       </c>
       <c r="E64" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="F64">
@@ -2709,7 +2936,7 @@
         <v>4</v>
       </c>
       <c r="J64" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>1.2039728043259361</v>
       </c>
     </row>

</xml_diff>

<commit_message>
01: Finished experimental part
</commit_message>
<xml_diff>
--- a/01_Townsend/data/Townsend.xlsx
+++ b/01_Townsend/data/Townsend.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\Škola Mgr\Praktikum plazma\PraktikaPlazma\01_Townsend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B44060C-96FB-43AB-AD6B-41F73FEC4053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEFFA44-1E22-4C50-83AB-98ACC0BD792C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="2850" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12540" yWindow="3105" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="41">
   <si>
     <t>Vcm-1</t>
   </si>
@@ -148,6 +148,15 @@
   </si>
   <si>
     <t>error</t>
+  </si>
+  <si>
+    <t>relative error</t>
+  </si>
+  <si>
+    <t>U Ar [eV]</t>
+  </si>
+  <si>
+    <t>přesnější, viz error</t>
   </si>
 </sst>
 </file>
@@ -552,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z64"/>
+  <dimension ref="A1:AA64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,6 +573,7 @@
     <col min="12" max="12" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" customWidth="1"/>
     <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12.140625" customWidth="1"/>
   </cols>
@@ -1244,7 +1254,7 @@
         <v>1.6993199999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>A16+2</f>
         <v>87</v>
@@ -1300,7 +1310,7 @@
         <v>19.918209999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ref="A18:A25" si="9">A17+2</f>
         <v>89</v>
@@ -1356,7 +1366,7 @@
         <v>1.22679</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="9"/>
         <v>91</v>
@@ -1412,7 +1422,7 @@
         <v>7.0880000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="9"/>
         <v>93</v>
@@ -1468,7 +1478,7 @@
         <v>0.48057</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="9"/>
         <v>95</v>
@@ -1503,7 +1513,7 @@
       </c>
       <c r="T21" s="3"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="9"/>
         <v>97</v>
@@ -1567,7 +1577,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="9"/>
         <v>99</v>
@@ -1639,7 +1649,7 @@
         <v>9.9375000000000002E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="9"/>
         <v>101</v>
@@ -1711,7 +1721,7 @@
         <v>8.8333333333333337E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="9"/>
         <v>103</v>
@@ -1783,7 +1793,7 @@
         <v>7.9500000000000005E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="L26" s="3">
         <v>11000</v>
       </c>
@@ -1823,7 +1833,7 @@
         <v>7.2272727272727271E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>0</v>
       </c>
@@ -1872,7 +1882,7 @@
         <v>6.6249999999999998E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1889,7 +1899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>85</f>
         <v>85</v>
@@ -1955,7 +1965,7 @@
         <v>9.3113119525302359</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>A29+2</f>
         <v>87</v>
@@ -2002,6 +2012,13 @@
         <f>EXP(N30)</f>
         <v>1.1764012614570987</v>
       </c>
+      <c r="R30" t="s">
+        <v>38</v>
+      </c>
+      <c r="S30">
+        <f>Q30/Q29</f>
+        <v>0.10707347477895925</v>
+      </c>
       <c r="U30" s="3" t="s">
         <v>37</v>
       </c>
@@ -2015,8 +2032,15 @@
         <f>EXP(V30)</f>
         <v>1.1635899376508727</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z30" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA30">
+        <f>Y30/Y29</f>
+        <v>0.12496519755571944</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" ref="A31:A38" si="20">A30+2</f>
         <v>89</v>
@@ -2077,7 +2101,7 @@
         <v>156.39938000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="20"/>
         <v>91</v>
@@ -2123,6 +2147,13 @@
       <c r="Q32">
         <v>19.8</v>
       </c>
+      <c r="R32" t="s">
+        <v>38</v>
+      </c>
+      <c r="S32">
+        <f>Q32/Q31</f>
+        <v>0.12428881531855884</v>
+      </c>
       <c r="U32" s="3" t="s">
         <v>37</v>
       </c>
@@ -2135,8 +2166,15 @@
       <c r="Y32">
         <v>18.478000000000002</v>
       </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z32" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA32">
+        <f>Y32/Y31</f>
+        <v>0.11814624840584406</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="20"/>
         <v>93</v>
@@ -2184,7 +2222,7 @@
         <v>16.796707144743483</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="20"/>
         <v>95</v>
@@ -2217,8 +2255,36 @@
         <f t="shared" si="19"/>
         <v>5.6300163244165917</v>
       </c>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="P34" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q34">
+        <f>Q33*S34</f>
+        <v>2.378680340093053</v>
+      </c>
+      <c r="R34" t="s">
+        <v>38</v>
+      </c>
+      <c r="S34">
+        <f>SQRT((S30^2)+(S32^2))</f>
+        <v>0.16405011007168283</v>
+      </c>
+      <c r="X34" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y34">
+        <f>Y33*AA34</f>
+        <v>2.8885861676856535</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA34">
+        <f>SQRT((AA30^2)+(AA32^2))</f>
+        <v>0.17197336018266143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="20"/>
         <v>97</v>
@@ -2252,7 +2318,7 @@
         <v>5.2346673394715806</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="20"/>
         <v>99</v>
@@ -2285,8 +2351,22 @@
         <f t="shared" si="19"/>
         <v>4.7957905455967413</v>
       </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="N36" t="s">
+        <v>39</v>
+      </c>
+      <c r="O36">
+        <v>15.76</v>
+      </c>
+      <c r="Q36">
+        <f>O36-Q33</f>
+        <v>1.260281962299981</v>
+      </c>
+      <c r="Y36">
+        <f>Y33-O36</f>
+        <v>1.0367071447434828</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="20"/>
         <v>101</v>
@@ -2319,8 +2399,11 @@
         <f t="shared" si="19"/>
         <v>4.2766661190160553</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="20"/>
         <v>103</v>
@@ -2354,7 +2437,7 @@
         <v>3.5165082281731497</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>0</v>
       </c>
@@ -2365,7 +2448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -2382,7 +2465,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42">
         <f>85</f>
         <v>85</v>
@@ -2416,7 +2499,7 @@
         <v>7.5504859736280663</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43">
         <f>A42+2</f>
         <v>87</v>
@@ -2450,7 +2533,7 @@
         <v>7.1258192845530486</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" ref="A44:A51" si="24">A43+2</f>
         <v>89</v>
@@ -2484,7 +2567,7 @@
         <v>6.6665326142680215</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="24"/>
         <v>91</v>
@@ -2518,7 +2601,7 @@
         <v>6.1696107324914564</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="24"/>
         <v>93</v>
@@ -2552,7 +2635,7 @@
         <v>5.7104270173748697</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="24"/>
         <v>95</v>
@@ -2586,7 +2669,7 @@
         <v>5.1984970312658261</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="24"/>
         <v>97</v>

</xml_diff>

<commit_message>
01: Téměř hotová verze první opravy podle doktoranda, dodělat pevné mezery a zkontrolovat
</commit_message>
<xml_diff>
--- a/01_Townsend/data/Townsend.xlsx
+++ b/01_Townsend/data/Townsend.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\Škola Mgr\Praktikum plazma\PraktikaPlazma\01_Townsend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBE821A-CBBC-4D13-84FA-DFCD8E8A0AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3C4333-5102-41B4-A0C8-D300E7816DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14475" yWindow="2910" windowWidth="14415" windowHeight="9120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -216,13 +216,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -563,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Y32" sqref="Y32"/>
+    <sheetView tabSelected="1" topLeftCell="N24" workbookViewId="0">
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,23 +1404,23 @@
         <v>120</v>
       </c>
       <c r="M19">
-        <v>3.2299899999999999</v>
+        <v>2.91371</v>
       </c>
       <c r="N19">
-        <v>1.3170500000000001</v>
+        <v>1.7809200000000001</v>
       </c>
       <c r="Q19">
         <f t="shared" si="5"/>
-        <v>3.7323945567549304</v>
+        <v>5.9353143967812478</v>
       </c>
       <c r="T19" s="3">
         <v>120</v>
       </c>
       <c r="U19">
-        <v>2.7830599999999999</v>
+        <v>2.7817500000000002</v>
       </c>
       <c r="Y19">
-        <v>7.0880000000000001</v>
+        <v>7.1057199999999998</v>
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
@@ -1459,23 +1460,23 @@
         <v>24</v>
       </c>
       <c r="M20">
-        <v>0.20183999999999999</v>
+        <v>0.10781</v>
       </c>
       <c r="N20">
-        <v>0.25047999999999998</v>
+        <v>0.14085</v>
       </c>
       <c r="Q20">
         <f t="shared" si="5"/>
-        <v>1.2846418968311495</v>
+        <v>1.1512519472404261</v>
       </c>
       <c r="T20" s="3" t="s">
         <v>24</v>
       </c>
       <c r="U20">
-        <v>3.5029999999999999E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="Y20">
-        <v>0.48057</v>
+        <v>0.501</v>
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
@@ -1880,15 +1881,15 @@
       </c>
       <c r="M27">
         <f>M19*100</f>
-        <v>322.99899999999997</v>
+        <v>291.37099999999998</v>
       </c>
       <c r="N27">
         <f t="shared" si="10"/>
-        <v>4.0628805031446538</v>
+        <v>3.6650440251572323</v>
       </c>
       <c r="O27">
         <f t="shared" si="11"/>
-        <v>1.4018922055823455</v>
+        <v>1.2988403475876769</v>
       </c>
       <c r="P27">
         <f t="shared" si="12"/>
@@ -1903,15 +1904,15 @@
       </c>
       <c r="U27">
         <f>U19*100</f>
-        <v>278.30599999999998</v>
+        <v>278.17500000000001</v>
       </c>
       <c r="V27">
         <f t="shared" si="14"/>
-        <v>3.5007044025157232</v>
+        <v>3.4990566037735849</v>
       </c>
       <c r="W27">
         <f t="shared" si="15"/>
-        <v>1.2529642061073567</v>
+        <v>1.2524933903834781</v>
       </c>
       <c r="X27">
         <f t="shared" si="16"/>
@@ -1979,14 +1980,14 @@
         <v>35</v>
       </c>
       <c r="N29">
-        <v>2.3967000000000001</v>
+        <v>2.1948500000000002</v>
       </c>
       <c r="P29" t="s">
         <v>19</v>
       </c>
       <c r="Q29">
         <f>EXP(N29)</f>
-        <v>10.986859853811996</v>
+        <v>8.9786541576808094</v>
       </c>
       <c r="T29" t="s">
         <v>34</v>
@@ -1995,14 +1996,14 @@
         <v>35</v>
       </c>
       <c r="V29">
-        <v>2.23123</v>
+        <v>2.2303099999999998</v>
       </c>
       <c r="X29" t="s">
         <v>19</v>
       </c>
       <c r="Y29">
         <f>EXP(V29)</f>
-        <v>9.3113119525302359</v>
+        <v>9.302749484872967</v>
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
@@ -2043,41 +2044,41 @@
         <v>37</v>
       </c>
       <c r="N30">
-        <v>0.16245999999999999</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="P30" s="3" t="s">
         <v>37</v>
       </c>
       <c r="Q30">
         <f>EXP(N30)</f>
-        <v>1.1764012614570987</v>
+        <v>1.0470744109569372</v>
       </c>
       <c r="R30" t="s">
         <v>38</v>
       </c>
       <c r="S30">
         <f>Q30/Q29</f>
-        <v>0.10707347477895925</v>
+        <v>0.11661819160962059</v>
       </c>
       <c r="U30" s="3" t="s">
         <v>37</v>
       </c>
       <c r="V30">
-        <v>0.15151000000000001</v>
+        <v>0.15090000000000001</v>
       </c>
       <c r="X30" s="3" t="s">
         <v>37</v>
       </c>
       <c r="Y30">
         <f>EXP(V30)</f>
-        <v>1.1635899376508727</v>
+        <v>1.1628803642308014</v>
       </c>
       <c r="Z30" t="s">
         <v>38</v>
       </c>
       <c r="AA30">
         <f>Y30/Y29</f>
-        <v>0.12496519755571944</v>
+        <v>0.12500394277216001</v>
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
@@ -2118,27 +2119,27 @@
         <v>36</v>
       </c>
       <c r="N31">
-        <v>-159.30636999999999</v>
+        <v>-0.13697000000000001</v>
       </c>
       <c r="P31" t="s">
         <v>20</v>
       </c>
       <c r="Q31">
-        <f>N31*-1</f>
-        <v>159.30636999999999</v>
+        <f>N31*-1*1000</f>
+        <v>136.97</v>
       </c>
       <c r="U31" t="s">
         <v>36</v>
       </c>
       <c r="V31">
-        <v>-156.39938000000001</v>
+        <v>-0.15629999999999999</v>
       </c>
       <c r="X31" t="s">
         <v>20</v>
       </c>
       <c r="Y31">
-        <f>V31*-1</f>
-        <v>156.39938000000001</v>
+        <f>V31*-1*1000</f>
+        <v>156.29999999999998</v>
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
@@ -2179,39 +2180,41 @@
         <v>37</v>
       </c>
       <c r="N32">
-        <v>19.8</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="P32" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Q32">
-        <v>19.8</v>
+      <c r="Q32" s="6">
+        <f>N32*1000</f>
+        <v>5</v>
       </c>
       <c r="R32" t="s">
         <v>38</v>
       </c>
       <c r="S32">
         <f>Q32/Q31</f>
-        <v>0.12428881531855884</v>
+        <v>3.6504344016938015E-2</v>
       </c>
       <c r="U32" s="3" t="s">
         <v>37</v>
       </c>
       <c r="V32">
-        <v>18.478000000000002</v>
+        <v>1.8409999999999999E-2</v>
       </c>
       <c r="X32" s="3" t="s">
         <v>37</v>
       </c>
       <c r="Y32">
-        <v>18.478000000000002</v>
+        <f>V32*1000</f>
+        <v>18.41</v>
       </c>
       <c r="Z32" t="s">
         <v>38</v>
       </c>
       <c r="AA32">
         <f>Y32/Y31</f>
-        <v>0.11814624840584406</v>
+        <v>0.117786308381318</v>
       </c>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
@@ -2252,14 +2255,14 @@
       </c>
       <c r="Q33" s="1">
         <f>Q31/Q29</f>
-        <v>14.499718037700019</v>
+        <v>15.255070258255655</v>
       </c>
       <c r="X33" s="1" t="s">
         <v>22</v>
       </c>
       <c r="Y33" s="1">
         <f>Y31/Y29</f>
-        <v>16.796707144743483</v>
+        <v>16.80148436267757</v>
       </c>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
@@ -2300,28 +2303,28 @@
       </c>
       <c r="Q34">
         <f>Q33*S34</f>
-        <v>2.378680340093053</v>
+        <v>1.8641402328251779</v>
       </c>
       <c r="R34" t="s">
         <v>38</v>
       </c>
       <c r="S34">
         <f>SQRT((S30^2)+(S32^2))</f>
-        <v>0.16405011007168283</v>
+        <v>0.12219807587030632</v>
       </c>
       <c r="X34" s="3" t="s">
         <v>37</v>
       </c>
       <c r="Y34">
         <f>Y33*AA34</f>
-        <v>2.8885861676856535</v>
+        <v>2.8857301488306701</v>
       </c>
       <c r="Z34" t="s">
         <v>38</v>
       </c>
       <c r="AA34">
         <f>SQRT((AA30^2)+(AA32^2))</f>
-        <v>0.17197336018266143</v>
+        <v>0.17175447636287211</v>
       </c>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
@@ -2399,11 +2402,11 @@
       </c>
       <c r="Q36">
         <f>O36-Q33</f>
-        <v>1.260281962299981</v>
+        <v>0.5049297417443448</v>
       </c>
       <c r="Y36">
         <f>Y33-O36</f>
-        <v>1.0367071447434828</v>
+        <v>1.0414843626775703</v>
       </c>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
01: Correction in progress
</commit_message>
<xml_diff>
--- a/01_Townsend/data/Townsend.xlsx
+++ b/01_Townsend/data/Townsend.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\Škola Mgr\Praktikum plazma\PraktikaPlazma\01_Townsend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3C4333-5102-41B4-A0C8-D300E7816DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A7D2FB-B895-4B68-84F8-84FC102BFE77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14475" yWindow="2910" windowWidth="14415" windowHeight="9120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="78">
   <si>
     <t>Vcm-1</t>
   </si>
@@ -157,6 +157,117 @@
   </si>
   <si>
     <t>přesnější, viz error</t>
+  </si>
+  <si>
+    <t>i A</t>
+  </si>
+  <si>
+    <t>ln I z i [A]</t>
+  </si>
+  <si>
+    <t>Equation</t>
+  </si>
+  <si>
+    <t>Plot</t>
+  </si>
+  <si>
+    <t>R-Square (COD)</t>
+  </si>
+  <si>
+    <t>Adj. R-Square</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>ExpGro1</t>
+  </si>
+  <si>
+    <t>y = A1*exp(x/t1) + y0</t>
+  </si>
+  <si>
+    <t>y0</t>
+  </si>
+  <si>
+    <t>-17,71263 ± 0,96317</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>-9,69687 ± 0,78472</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>-1,52141 ± 0,29447</t>
+  </si>
+  <si>
+    <t>Reduced Chi-Sqr</t>
+  </si>
+  <si>
+    <t>-14,43886 ± 1,01438</t>
+  </si>
+  <si>
+    <t>-16,11527 ± 0,64138</t>
+  </si>
+  <si>
+    <t>-9,60771 ± 0,98565</t>
+  </si>
+  <si>
+    <t>-9,26102 ± 0,5943</t>
+  </si>
+  <si>
+    <t>-4,01068 ± 0,5527</t>
+  </si>
+  <si>
+    <t>-2,49289 ± 0,26295</t>
+  </si>
+  <si>
+    <t>100 Vcm\+(-1)</t>
+  </si>
+  <si>
+    <t>80 Vcm\+(-1)</t>
+  </si>
+  <si>
+    <t>120 Vcm\+(-1)</t>
+  </si>
+  <si>
+    <t>I posun</t>
+  </si>
+  <si>
+    <t>1/alpha</t>
+  </si>
+  <si>
+    <t>I0</t>
+  </si>
+  <si>
+    <t>90 Vcm\+(-1)</t>
+  </si>
+  <si>
+    <t>-16,75696 ± 0,81858</t>
+  </si>
+  <si>
+    <t>-7,90233 ± 0,75321</t>
+  </si>
+  <si>
+    <t>-2,38852 ± 0,38346</t>
+  </si>
+  <si>
+    <t>110 Vcm\+(-1)</t>
+  </si>
+  <si>
+    <t>-14,63026 ± 1,55229</t>
+  </si>
+  <si>
+    <t>-10,92251 ± 1,46892</t>
+  </si>
+  <si>
+    <t>-2,91704 ± 0,59548</t>
+  </si>
+  <si>
+    <t>alpha</t>
   </si>
 </sst>
 </file>
@@ -167,7 +278,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,16 +306,29 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -212,11 +336,170 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC0C0C0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC0C0C0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFC0C0C0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFC0C0C0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC0C0C0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -224,6 +507,54 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -564,19 +895,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N24" workbookViewId="0">
-      <selection activeCell="S33" sqref="S33"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="S58" sqref="S58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="9.140625" style="3"/>
     <col min="12" max="12" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.85546875" customWidth="1"/>
     <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12.140625" customWidth="1"/>
+    <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -616,8 +950,14 @@
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
       <c r="J2" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>9</v>
@@ -670,9 +1010,17 @@
       <c r="H3">
         <v>1642</v>
       </c>
+      <c r="I3">
+        <f>E3/1000000000000</f>
+        <v>1.6506666666666668E-9</v>
+      </c>
       <c r="J3" s="3">
         <f>LN(E3)</f>
         <v>7.4089345256963224</v>
+      </c>
+      <c r="K3" s="3">
+        <f>LN(I3)</f>
+        <v>-20.222086590232227</v>
       </c>
       <c r="L3" s="3">
         <v>80</v>
@@ -710,10 +1058,18 @@
       <c r="H4">
         <v>1139</v>
       </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I5" si="3">E4/1000000000000</f>
+        <v>1.111E-9</v>
+      </c>
       <c r="J4" s="3">
         <f>LN(E4)</f>
         <v>7.0130157896396303</v>
       </c>
+      <c r="K4" s="3">
+        <f t="shared" ref="K4:K64" si="4">LN(I4)</f>
+        <v>-20.61800532628892</v>
+      </c>
       <c r="L4" s="3">
         <v>90</v>
       </c>
@@ -723,7 +1079,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" ref="A5:A12" si="3">A4+2</f>
+        <f t="shared" ref="A5:A12" si="5">A4+2</f>
         <v>89</v>
       </c>
       <c r="B5" s="1">
@@ -750,9 +1106,17 @@
       <c r="H5">
         <v>735</v>
       </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>7.5133333333333332E-10</v>
+      </c>
       <c r="J5" s="3">
-        <f t="shared" ref="J5:J25" si="4">LN(E5)</f>
+        <f t="shared" ref="J5:J25" si="6">LN(E5)</f>
         <v>6.621849405931612</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="4"/>
+        <v>-21.009171709996938</v>
       </c>
       <c r="L5" s="3">
         <v>100</v>
@@ -763,7 +1127,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>91</v>
       </c>
       <c r="B6" s="1">
@@ -790,9 +1154,17 @@
       <c r="H6">
         <v>490</v>
       </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I64" si="7">E6/1000000000000</f>
+        <v>4.8266666666666665E-10</v>
+      </c>
       <c r="J6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.1793262842775523</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="4"/>
+        <v>-21.451694831650997</v>
       </c>
       <c r="L6" s="3">
         <v>110</v>
@@ -803,7 +1175,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>93</v>
       </c>
       <c r="B7" s="1">
@@ -830,9 +1202,17 @@
       <c r="H7">
         <v>323</v>
       </c>
+      <c r="I7">
+        <f t="shared" si="7"/>
+        <v>3.2466666666666668E-10</v>
+      </c>
       <c r="J7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.7827990149744251</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="4"/>
+        <v>-21.848222100954121</v>
       </c>
       <c r="L7" s="3">
         <v>120</v>
@@ -843,7 +1223,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>95</v>
       </c>
       <c r="B8" s="1">
@@ -870,9 +1250,17 @@
       <c r="H8">
         <v>198</v>
       </c>
+      <c r="I8">
+        <f t="shared" si="7"/>
+        <v>1.9733333333333335E-10</v>
+      </c>
       <c r="J8" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.2848943462158964</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="4"/>
+        <v>-22.346126769712651</v>
       </c>
       <c r="T8" t="s">
         <v>17</v>
@@ -880,7 +1268,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>97</v>
       </c>
       <c r="B9" s="1">
@@ -907,9 +1295,17 @@
       <c r="H9">
         <v>132</v>
       </c>
+      <c r="I9">
+        <f t="shared" si="7"/>
+        <v>1.2633333333333334E-10</v>
+      </c>
       <c r="J9" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.8389239164143163</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="4"/>
+        <v>-22.792097199514231</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>25</v>
@@ -920,7 +1316,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>99</v>
       </c>
       <c r="B10" s="1">
@@ -947,9 +1343,17 @@
       <c r="H10">
         <v>72</v>
       </c>
+      <c r="I10">
+        <f t="shared" si="7"/>
+        <v>7.4333333333333322E-11</v>
+      </c>
       <c r="J10" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.3085594827920088</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="4"/>
+        <v>-23.322461633136538</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>9</v>
@@ -993,7 +1397,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>101</v>
       </c>
       <c r="B11" s="1">
@@ -1020,9 +1424,17 @@
       <c r="H11">
         <v>41</v>
       </c>
+      <c r="I11">
+        <f t="shared" si="7"/>
+        <v>3.7666666666666666E-11</v>
+      </c>
       <c r="J11" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.6287755300442308</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="4"/>
+        <v>-24.002245585884317</v>
       </c>
       <c r="L11" s="3">
         <v>80</v>
@@ -1049,7 +1461,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>103</v>
       </c>
       <c r="B12" s="1">
@@ -1076,9 +1488,17 @@
       <c r="H12">
         <v>19</v>
       </c>
+      <c r="I12">
+        <f t="shared" si="7"/>
+        <v>1.8666666666666667E-11</v>
+      </c>
       <c r="J12" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.9267394020670396</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="4"/>
+        <v>-24.704281713861509</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>24</v>
@@ -1090,7 +1510,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="Q12">
-        <f t="shared" ref="Q12:Q20" si="5">EXP(N12)</f>
+        <f>EXP(N12)</f>
         <v>1.0554846021550801</v>
       </c>
       <c r="T12" s="3" t="s">
@@ -1114,7 +1534,7 @@
         <v>3.4063099999999999</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="5"/>
+        <f>EXP(N13)</f>
         <v>30.153771302174523</v>
       </c>
       <c r="T13" s="3">
@@ -1147,7 +1567,7 @@
         <v>0.1046</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="5"/>
+        <f>EXP(N14)</f>
         <v>1.1102664149565653</v>
       </c>
       <c r="T14" s="3" t="s">
@@ -1186,7 +1606,7 @@
         <v>2.7288800000000002</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="5"/>
+        <f>EXP(N15)</f>
         <v>15.315723799642379</v>
       </c>
       <c r="T15" s="3">
@@ -1212,7 +1632,7 @@
         <v>160</v>
       </c>
       <c r="D16">
-        <f t="shared" ref="D16:D25" si="6">C16/2</f>
+        <f t="shared" ref="D16:D25" si="8">C16/2</f>
         <v>80</v>
       </c>
       <c r="E16" s="2">
@@ -1228,9 +1648,17 @@
       <c r="H16">
         <v>1500</v>
       </c>
+      <c r="I16">
+        <f t="shared" si="7"/>
+        <v>1.5143333333333332E-9</v>
+      </c>
       <c r="J16" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.3227305770912938</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="4"/>
+        <v>-20.308290538837255</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>24</v>
@@ -1242,7 +1670,7 @@
         <v>0.11022</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="5"/>
+        <f>EXP(N16)</f>
         <v>1.1165236786502826</v>
       </c>
       <c r="T16" s="3" t="s">
@@ -1264,15 +1692,15 @@
         <v>1.8</v>
       </c>
       <c r="C17">
-        <f t="shared" ref="C17:C25" si="7">C$14*$B17</f>
+        <f t="shared" ref="C17:C25" si="9">C$14*$B17</f>
         <v>144</v>
       </c>
       <c r="D17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>72</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" ref="E17:E25" si="8">AVERAGE(F17,G17,H17)</f>
+        <f t="shared" ref="E17:E25" si="10">AVERAGE(F17,G17,H17)</f>
         <v>1201.6666666666667</v>
       </c>
       <c r="F17">
@@ -1284,9 +1712,17 @@
       <c r="H17">
         <v>1200</v>
       </c>
+      <c r="I17">
+        <f t="shared" si="7"/>
+        <v>1.2016666666666668E-9</v>
+      </c>
       <c r="J17" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.0914647610509398</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" si="4"/>
+        <v>-20.539556354877607</v>
       </c>
       <c r="L17" s="3">
         <v>110</v>
@@ -1298,7 +1734,7 @@
         <v>2.5054599999999998</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="5"/>
+        <f>EXP(N17)</f>
         <v>12.249192298492478</v>
       </c>
       <c r="T17" s="3">
@@ -1313,22 +1749,22 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" ref="A18:A25" si="9">A17+2</f>
+        <f t="shared" ref="A18:A25" si="11">A17+2</f>
         <v>89</v>
       </c>
       <c r="B18" s="1">
         <v>1.6</v>
       </c>
       <c r="C18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>128</v>
       </c>
       <c r="D18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>64</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>853</v>
       </c>
       <c r="F18">
@@ -1340,9 +1776,17 @@
       <c r="H18">
         <v>853</v>
       </c>
+      <c r="I18">
+        <f t="shared" si="7"/>
+        <v>8.5299999999999995E-10</v>
+      </c>
       <c r="J18" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.7487595474916793</v>
+      </c>
+      <c r="K18" s="3">
+        <f t="shared" si="4"/>
+        <v>-20.882261568436871</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>24</v>
@@ -1354,7 +1798,7 @@
         <v>0.10979</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="5"/>
+        <f>EXP(N18)</f>
         <v>1.1160436766762836</v>
       </c>
       <c r="T18" s="3" t="s">
@@ -1369,22 +1813,22 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>91</v>
       </c>
       <c r="B19" s="1">
         <v>1.4</v>
       </c>
       <c r="C19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>112</v>
       </c>
       <c r="D19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>56</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>622</v>
       </c>
       <c r="F19">
@@ -1396,9 +1840,17 @@
       <c r="H19">
         <v>626</v>
       </c>
+      <c r="I19">
+        <f t="shared" si="7"/>
+        <v>6.2200000000000002E-10</v>
+      </c>
       <c r="J19" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.4329400927391793</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" si="4"/>
+        <v>-21.198081023189367</v>
       </c>
       <c r="L19" s="3">
         <v>120</v>
@@ -1410,7 +1862,7 @@
         <v>1.7809200000000001</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="5"/>
+        <f>EXP(N19)</f>
         <v>5.9353143967812478</v>
       </c>
       <c r="T19" s="3">
@@ -1425,22 +1877,22 @@
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>93</v>
       </c>
       <c r="B20" s="1">
         <v>1.2</v>
       </c>
       <c r="C20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>96</v>
       </c>
       <c r="D20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>48</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>435.33333333333331</v>
       </c>
       <c r="F20">
@@ -1452,9 +1904,17 @@
       <c r="H20">
         <v>425</v>
       </c>
+      <c r="I20">
+        <f t="shared" si="7"/>
+        <v>4.3533333333333333E-10</v>
+      </c>
       <c r="J20" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.0761120211682664</v>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" si="4"/>
+        <v>-21.55490909476028</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>24</v>
@@ -1466,7 +1926,7 @@
         <v>0.14085</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="5"/>
+        <f>EXP(N20)</f>
         <v>1.1512519472404261</v>
       </c>
       <c r="T20" s="3" t="s">
@@ -1481,22 +1941,22 @@
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>95</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
       </c>
       <c r="C21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>80</v>
       </c>
       <c r="D21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>40</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>300.66666666666669</v>
       </c>
       <c r="F21">
@@ -1508,30 +1968,38 @@
       <c r="H21">
         <v>301</v>
       </c>
+      <c r="I21">
+        <f t="shared" si="7"/>
+        <v>3.0066666666666666E-10</v>
+      </c>
       <c r="J21" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.706002231394514</v>
+      </c>
+      <c r="K21" s="3">
+        <f t="shared" si="4"/>
+        <v>-21.925018884534033</v>
       </c>
       <c r="T21" s="3"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>97</v>
       </c>
       <c r="B22" s="1">
         <v>0.8</v>
       </c>
       <c r="C22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>64</v>
       </c>
       <c r="D22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>32</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>196</v>
       </c>
       <c r="F22">
@@ -1543,9 +2011,17 @@
       <c r="H22">
         <v>192</v>
       </c>
+      <c r="I22">
+        <f t="shared" si="7"/>
+        <v>1.96E-10</v>
+      </c>
       <c r="J22" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.2781146592305168</v>
+      </c>
+      <c r="K22" s="3">
+        <f t="shared" si="4"/>
+        <v>-22.35290645669803</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>31</v>
@@ -1580,22 +2056,22 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>99</v>
       </c>
       <c r="B23" s="1">
         <v>0.6</v>
       </c>
       <c r="C23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>48</v>
       </c>
       <c r="D23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>24</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>135</v>
       </c>
       <c r="F23">
@@ -1607,9 +2083,17 @@
       <c r="H23">
         <v>135</v>
       </c>
+      <c r="I23">
+        <f t="shared" si="7"/>
+        <v>1.35E-10</v>
+      </c>
       <c r="J23" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.9052747784384296</v>
+      </c>
+      <c r="K23" s="3">
+        <f t="shared" si="4"/>
+        <v>-22.725746337490119</v>
       </c>
       <c r="L23" s="3">
         <v>8000</v>
@@ -1660,22 +2144,22 @@
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>101</v>
       </c>
       <c r="B24" s="1">
         <v>0.4</v>
       </c>
       <c r="C24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>32</v>
       </c>
       <c r="D24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>92.666666666666671</v>
       </c>
       <c r="F24">
@@ -1687,9 +2171,17 @@
       <c r="H24">
         <v>96</v>
       </c>
+      <c r="I24">
+        <f t="shared" si="7"/>
+        <v>9.266666666666667E-11</v>
+      </c>
       <c r="J24" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.5290088250225278</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" si="4"/>
+        <v>-23.102012290906021</v>
       </c>
       <c r="L24" s="3">
         <v>9000</v>
@@ -1699,19 +2191,19 @@
         <v>212.39699999999999</v>
       </c>
       <c r="N24">
-        <f t="shared" ref="N24:N27" si="10">M24/$L$1</f>
+        <f t="shared" ref="N24:N27" si="12">M24/$L$1</f>
         <v>2.6716603773584904</v>
       </c>
       <c r="O24">
-        <f t="shared" ref="O24:O27" si="11">LN(N24)</f>
+        <f t="shared" ref="O24:O27" si="13">LN(N24)</f>
         <v>0.98270014331396338</v>
       </c>
       <c r="P24">
-        <f t="shared" ref="P24:P27" si="12">$L$1/L24</f>
+        <f t="shared" ref="P24:P27" si="14">$L$1/L24</f>
         <v>8.8333333333333337E-3</v>
       </c>
       <c r="Q24">
-        <f t="shared" ref="Q24:Q27" si="13">P24*1000</f>
+        <f>P24*1000</f>
         <v>8.8333333333333339</v>
       </c>
       <c r="T24" s="3">
@@ -1722,40 +2214,40 @@
         <v>185.24799999999999</v>
       </c>
       <c r="V24">
-        <f t="shared" ref="V24:V27" si="14">U24/$L$1</f>
+        <f t="shared" ref="V24:V27" si="15">U24/$L$1</f>
         <v>2.3301635220125787</v>
       </c>
       <c r="W24">
-        <f t="shared" ref="W24:W27" si="15">LN(V24)</f>
+        <f t="shared" ref="W24:W27" si="16">LN(V24)</f>
         <v>0.84593844623630798</v>
       </c>
       <c r="X24">
-        <f t="shared" ref="X24:X27" si="16">$L$1/T24</f>
+        <f t="shared" ref="X24:X27" si="17">$L$1/T24</f>
         <v>8.8333333333333337E-3</v>
       </c>
       <c r="Y24">
-        <f t="shared" ref="Y24:Y27" si="17">X24*1000</f>
+        <f t="shared" ref="Y24:Y27" si="18">X24*1000</f>
         <v>8.8333333333333339</v>
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>103</v>
       </c>
       <c r="B25" s="1">
         <v>0.2</v>
       </c>
       <c r="C25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="D25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>57.333333333333336</v>
       </c>
       <c r="F25">
@@ -1767,9 +2259,17 @@
       <c r="H25">
         <v>61</v>
       </c>
+      <c r="I25">
+        <f t="shared" si="7"/>
+        <v>5.7333333333333336E-11</v>
+      </c>
       <c r="J25" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.0488821881453436</v>
+      </c>
+      <c r="K25" s="3">
+        <f t="shared" si="4"/>
+        <v>-23.582138927783205</v>
       </c>
       <c r="L25" s="3">
         <v>10000</v>
@@ -1779,19 +2279,19 @@
         <v>242.773</v>
       </c>
       <c r="N25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3.0537484276729558</v>
       </c>
       <c r="O25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.1163698287056711</v>
       </c>
       <c r="P25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>7.9500000000000005E-3</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="13"/>
+        <f>P25*1000</f>
         <v>7.95</v>
       </c>
       <c r="T25" s="3">
@@ -1802,19 +2302,19 @@
         <v>206.71499999999997</v>
       </c>
       <c r="V25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.6001886792452829</v>
       </c>
       <c r="W25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.95558401133493154</v>
       </c>
       <c r="X25">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>7.9500000000000005E-3</v>
       </c>
       <c r="Y25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>7.95</v>
       </c>
     </row>
@@ -1827,19 +2327,19 @@
         <v>259.81700000000001</v>
       </c>
       <c r="N26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3.2681383647798743</v>
       </c>
       <c r="O26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.1842205153854015</v>
       </c>
       <c r="P26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>7.2272727272727271E-3</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="13"/>
+        <f>P26*1000</f>
         <v>7.2272727272727275</v>
       </c>
       <c r="T26" s="3">
@@ -1854,15 +2354,15 @@
         <v>2.8730062893081763</v>
       </c>
       <c r="W26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.0553589691030669</v>
       </c>
       <c r="X26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>7.2272727272727271E-3</v>
       </c>
       <c r="Y26">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>7.2272727272727275</v>
       </c>
     </row>
@@ -1884,19 +2384,19 @@
         <v>291.37099999999998</v>
       </c>
       <c r="N27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3.6650440251572323</v>
       </c>
       <c r="O27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.2988403475876769</v>
       </c>
       <c r="P27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>6.6249999999999998E-3</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="13"/>
+        <f>P27*1000</f>
         <v>6.625</v>
       </c>
       <c r="T27" s="3">
@@ -1907,19 +2407,19 @@
         <v>278.17500000000001</v>
       </c>
       <c r="V27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3.4990566037735849</v>
       </c>
       <c r="W27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.2524933903834781</v>
       </c>
       <c r="X27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>6.6249999999999998E-3</v>
       </c>
       <c r="Y27">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.625</v>
       </c>
     </row>
@@ -1953,7 +2453,7 @@
         <v>180</v>
       </c>
       <c r="D29">
-        <f t="shared" ref="D29:D38" si="18">C29/2</f>
+        <f t="shared" ref="D29:D38" si="19">C29/2</f>
         <v>90</v>
       </c>
       <c r="E29" s="2">
@@ -1969,9 +2469,17 @@
       <c r="H29">
         <v>1844</v>
       </c>
+      <c r="I29">
+        <f t="shared" si="7"/>
+        <v>1.842E-9</v>
+      </c>
       <c r="J29" s="3">
         <f>LN(E29)</f>
         <v>7.5186072168152522</v>
+      </c>
+      <c r="K29" s="3">
+        <f t="shared" si="4"/>
+        <v>-20.112413899113296</v>
       </c>
       <c r="L29" t="s">
         <v>34</v>
@@ -2015,15 +2523,15 @@
         <v>1.8</v>
       </c>
       <c r="C30">
-        <f t="shared" ref="C30:C38" si="19">C$27*$B30</f>
+        <f t="shared" ref="C30:C38" si="20">C$27*$B30</f>
         <v>162</v>
       </c>
       <c r="D30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>81</v>
       </c>
       <c r="E30" s="2">
-        <f t="shared" ref="E30:E38" si="20">AVERAGE(F30,G30,H30)</f>
+        <f t="shared" ref="E30:E38" si="21">AVERAGE(F30,G30,H30)</f>
         <v>1247.6666666666667</v>
       </c>
       <c r="F30">
@@ -2035,9 +2543,17 @@
       <c r="H30">
         <v>1235</v>
       </c>
+      <c r="I30">
+        <f t="shared" si="7"/>
+        <v>1.2476666666666668E-9</v>
+      </c>
       <c r="J30" s="3">
-        <f t="shared" ref="J30:J64" si="21">LN(E30)</f>
+        <f t="shared" ref="J30:J64" si="22">LN(E30)</f>
         <v>7.1290304192363196</v>
+      </c>
+      <c r="K30" s="3">
+        <f t="shared" si="4"/>
+        <v>-20.501990696692229</v>
       </c>
       <c r="L30"/>
       <c r="M30" s="3" t="s">
@@ -2083,22 +2599,22 @@
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" ref="A31:A38" si="22">A30+2</f>
+        <f t="shared" ref="A31:A38" si="23">A30+2</f>
         <v>89</v>
       </c>
       <c r="B31" s="1">
         <v>1.6</v>
       </c>
       <c r="C31">
+        <f t="shared" si="20"/>
+        <v>144</v>
+      </c>
+      <c r="D31">
         <f t="shared" si="19"/>
-        <v>144</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="18"/>
         <v>72</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>898.66666666666663</v>
       </c>
       <c r="F31">
@@ -2110,9 +2626,17 @@
       <c r="H31">
         <v>901</v>
       </c>
+      <c r="I31">
+        <f t="shared" si="7"/>
+        <v>8.9866666666666667E-10</v>
+      </c>
       <c r="J31" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>6.8009121833640878</v>
+      </c>
+      <c r="K31" s="3">
+        <f t="shared" si="4"/>
+        <v>-20.83010893256446</v>
       </c>
       <c r="L31"/>
       <c r="M31" t="s">
@@ -2144,22 +2668,22 @@
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>91</v>
       </c>
       <c r="B32" s="1">
         <v>1.4</v>
       </c>
       <c r="C32">
+        <f t="shared" si="20"/>
+        <v>125.99999999999999</v>
+      </c>
+      <c r="D32">
         <f t="shared" si="19"/>
-        <v>125.99999999999999</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="18"/>
         <v>62.999999999999993</v>
       </c>
       <c r="E32" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>629.33333333333337</v>
       </c>
       <c r="F32">
@@ -2171,9 +2695,17 @@
       <c r="H32">
         <v>635</v>
       </c>
+      <c r="I32">
+        <f t="shared" si="7"/>
+        <v>6.2933333333333333E-10</v>
+      </c>
       <c r="J32" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>6.4446610580373367</v>
+      </c>
+      <c r="K32" s="3">
+        <f t="shared" si="4"/>
+        <v>-21.186360057891211</v>
       </c>
       <c r="L32"/>
       <c r="M32" s="3" t="s">
@@ -2219,22 +2751,22 @@
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>93</v>
       </c>
       <c r="B33" s="1">
         <v>1.2</v>
       </c>
       <c r="C33">
+        <f t="shared" si="20"/>
+        <v>108</v>
+      </c>
+      <c r="D33">
         <f t="shared" si="19"/>
-        <v>108</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="18"/>
         <v>54</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>437</v>
       </c>
       <c r="F33">
@@ -2246,9 +2778,17 @@
       <c r="H33">
         <v>444</v>
       </c>
+      <c r="I33">
+        <f t="shared" si="7"/>
+        <v>4.3699999999999999E-10</v>
+      </c>
       <c r="J33" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>6.0799331950955899</v>
+      </c>
+      <c r="K33" s="3">
+        <f t="shared" si="4"/>
+        <v>-21.551087920832959</v>
       </c>
       <c r="P33" s="1" t="s">
         <v>22</v>
@@ -2267,22 +2807,22 @@
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>95</v>
       </c>
       <c r="B34" s="1">
         <v>1</v>
       </c>
       <c r="C34">
+        <f t="shared" si="20"/>
+        <v>90</v>
+      </c>
+      <c r="D34">
         <f t="shared" si="19"/>
-        <v>90</v>
-      </c>
-      <c r="D34">
-        <f t="shared" si="18"/>
         <v>45</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>278.66666666666669</v>
       </c>
       <c r="F34">
@@ -2294,9 +2834,17 @@
       <c r="H34">
         <v>276</v>
       </c>
+      <c r="I34">
+        <f t="shared" si="7"/>
+        <v>2.7866666666666669E-10</v>
+      </c>
       <c r="J34" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>5.6300163244165917</v>
+      </c>
+      <c r="K34" s="3">
+        <f t="shared" si="4"/>
+        <v>-22.001004791511956</v>
       </c>
       <c r="P34" s="3" t="s">
         <v>37</v>
@@ -2329,22 +2877,22 @@
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>97</v>
       </c>
       <c r="B35" s="1">
         <v>0.8</v>
       </c>
       <c r="C35">
+        <f t="shared" si="20"/>
+        <v>72</v>
+      </c>
+      <c r="D35">
         <f t="shared" si="19"/>
-        <v>72</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="18"/>
         <v>36</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>187.66666666666666</v>
       </c>
       <c r="F35">
@@ -2356,29 +2904,37 @@
       <c r="H35">
         <v>188</v>
       </c>
+      <c r="I35">
+        <f t="shared" si="7"/>
+        <v>1.8766666666666666E-10</v>
+      </c>
       <c r="J35" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>5.2346673394715806</v>
+      </c>
+      <c r="K35" s="3">
+        <f t="shared" si="4"/>
+        <v>-22.396353776456966</v>
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>99</v>
       </c>
       <c r="B36" s="1">
         <v>0.6</v>
       </c>
       <c r="C36">
+        <f t="shared" si="20"/>
+        <v>54</v>
+      </c>
+      <c r="D36">
         <f t="shared" si="19"/>
-        <v>54</v>
-      </c>
-      <c r="D36">
-        <f t="shared" si="18"/>
         <v>27</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>121</v>
       </c>
       <c r="F36">
@@ -2390,9 +2946,17 @@
       <c r="H36">
         <v>119</v>
       </c>
+      <c r="I36">
+        <f t="shared" si="7"/>
+        <v>1.21E-10</v>
+      </c>
       <c r="J36" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>4.7957905455967413</v>
+      </c>
+      <c r="K36" s="3">
+        <f t="shared" si="4"/>
+        <v>-22.835230570331806</v>
       </c>
       <c r="N36" t="s">
         <v>39</v>
@@ -2411,22 +2975,22 @@
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>101</v>
       </c>
       <c r="B37" s="1">
         <v>0.4</v>
       </c>
       <c r="C37">
+        <f t="shared" si="20"/>
+        <v>36</v>
+      </c>
+      <c r="D37">
         <f t="shared" si="19"/>
-        <v>36</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="18"/>
         <v>18</v>
       </c>
       <c r="E37" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>72</v>
       </c>
       <c r="F37">
@@ -2438,9 +3002,17 @@
       <c r="H37">
         <v>72</v>
       </c>
+      <c r="I37">
+        <f t="shared" si="7"/>
+        <v>7.1999999999999997E-11</v>
+      </c>
       <c r="J37" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>4.2766661190160553</v>
+      </c>
+      <c r="K37" s="3">
+        <f t="shared" si="4"/>
+        <v>-23.354354996912495</v>
       </c>
       <c r="Q37" t="s">
         <v>40</v>
@@ -2448,22 +3020,22 @@
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>103</v>
       </c>
       <c r="B38" s="1">
         <v>0.2</v>
       </c>
       <c r="C38">
+        <f t="shared" si="20"/>
+        <v>18</v>
+      </c>
+      <c r="D38">
         <f t="shared" si="19"/>
-        <v>18</v>
-      </c>
-      <c r="D38">
-        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="E38" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33.666666666666664</v>
       </c>
       <c r="F38">
@@ -2475,9 +3047,17 @@
       <c r="H38">
         <v>32</v>
       </c>
+      <c r="I38">
+        <f t="shared" si="7"/>
+        <v>3.3666666666666667E-11</v>
+      </c>
       <c r="J38" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>3.5165082281731497</v>
+      </c>
+      <c r="K38" s="3">
+        <f t="shared" si="4"/>
+        <v>-24.114512887755399</v>
       </c>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
@@ -2521,7 +3101,7 @@
         <v>220</v>
       </c>
       <c r="D42">
-        <f t="shared" ref="D42:D51" si="23">C42/2</f>
+        <f t="shared" ref="D42:D51" si="24">C42/2</f>
         <v>110</v>
       </c>
       <c r="E42" s="2">
@@ -2537,9 +3117,17 @@
       <c r="H42">
         <v>1895</v>
       </c>
+      <c r="I42">
+        <f t="shared" si="7"/>
+        <v>1.9016666666666668E-9</v>
+      </c>
       <c r="J42" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>7.5504859736280663</v>
+      </c>
+      <c r="K42" s="3">
+        <f t="shared" si="4"/>
+        <v>-20.08053514230048</v>
       </c>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
@@ -2551,15 +3139,15 @@
         <v>1.8</v>
       </c>
       <c r="C43">
-        <f t="shared" ref="C43:C51" si="24">C$40*$B43</f>
+        <f t="shared" ref="C43:C51" si="25">C$40*$B43</f>
         <v>198</v>
       </c>
       <c r="D43">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>99</v>
       </c>
       <c r="E43" s="2">
-        <f t="shared" ref="E43:E51" si="25">AVERAGE(F43,G43,H43)</f>
+        <f t="shared" ref="E43:E51" si="26">AVERAGE(F43,G43,H43)</f>
         <v>1243.6666666666667</v>
       </c>
       <c r="F43">
@@ -2571,29 +3159,45 @@
       <c r="H43">
         <v>1241</v>
       </c>
+      <c r="I43">
+        <f t="shared" si="7"/>
+        <v>1.2436666666666668E-9</v>
+      </c>
       <c r="J43" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>7.1258192845530486</v>
       </c>
-    </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K43" s="3">
+        <f t="shared" si="4"/>
+        <v>-20.505201831375501</v>
+      </c>
+      <c r="M43" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N43" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="O43" s="14"/>
+      <c r="P43" s="16"/>
+    </row>
+    <row r="44" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" ref="A44:A51" si="26">A43+2</f>
+        <f t="shared" ref="A44:A51" si="27">A43+2</f>
         <v>89</v>
       </c>
       <c r="B44" s="1">
         <v>1.6</v>
       </c>
       <c r="C44">
+        <f t="shared" si="25"/>
+        <v>176</v>
+      </c>
+      <c r="D44">
         <f t="shared" si="24"/>
-        <v>176</v>
-      </c>
-      <c r="D44">
-        <f t="shared" si="23"/>
         <v>88</v>
       </c>
       <c r="E44" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>785.66666666666663</v>
       </c>
       <c r="F44">
@@ -2605,29 +3209,45 @@
       <c r="H44">
         <v>789</v>
       </c>
+      <c r="I44">
+        <f t="shared" si="7"/>
+        <v>7.8566666666666664E-10</v>
+      </c>
       <c r="J44" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>6.6665326142680215</v>
       </c>
-    </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K44" s="3">
+        <f t="shared" si="4"/>
+        <v>-20.964488501660526</v>
+      </c>
+      <c r="M44" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="N44" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="O44" s="18"/>
+      <c r="P44" s="19"/>
+    </row>
+    <row r="45" spans="1:27" ht="24" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>91</v>
       </c>
       <c r="B45" s="1">
         <v>1.4</v>
       </c>
       <c r="C45">
+        <f t="shared" si="25"/>
+        <v>154</v>
+      </c>
+      <c r="D45">
         <f t="shared" si="24"/>
-        <v>154</v>
-      </c>
-      <c r="D45">
-        <f t="shared" si="23"/>
         <v>77</v>
       </c>
       <c r="E45" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>478</v>
       </c>
       <c r="F45">
@@ -2639,29 +3259,67 @@
       <c r="H45">
         <v>477</v>
       </c>
+      <c r="I45">
+        <f t="shared" si="7"/>
+        <v>4.78E-10</v>
+      </c>
       <c r="J45" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>6.1696107324914564</v>
       </c>
-    </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K45" s="3">
+        <f t="shared" si="4"/>
+        <v>-21.461410383437091</v>
+      </c>
+      <c r="M45" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="N45" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="O45" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="P45" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="R45">
+        <v>80</v>
+      </c>
+      <c r="S45">
+        <v>100</v>
+      </c>
+      <c r="T45">
+        <v>120</v>
+      </c>
+      <c r="V45">
+        <v>80</v>
+      </c>
+      <c r="W45">
+        <v>100</v>
+      </c>
+      <c r="X45">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" ht="24" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>93</v>
       </c>
       <c r="B46" s="1">
         <v>1.2</v>
       </c>
       <c r="C46">
+        <f t="shared" si="25"/>
+        <v>132</v>
+      </c>
+      <c r="D46">
         <f t="shared" si="24"/>
-        <v>132</v>
-      </c>
-      <c r="D46">
-        <f t="shared" si="23"/>
         <v>66</v>
       </c>
       <c r="E46" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>302</v>
       </c>
       <c r="F46">
@@ -2673,29 +3331,73 @@
       <c r="H46">
         <v>297</v>
       </c>
+      <c r="I46">
+        <f t="shared" si="7"/>
+        <v>3.0199999999999999E-10</v>
+      </c>
       <c r="J46" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>5.7104270173748697</v>
       </c>
-    </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K46" s="3">
+        <f t="shared" si="4"/>
+        <v>-21.920594098553678</v>
+      </c>
+      <c r="M46" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="N46" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="O46" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="P46" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q46" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="R46">
+        <v>-14.43886</v>
+      </c>
+      <c r="S46">
+        <v>-16.115269999999999</v>
+      </c>
+      <c r="T46">
+        <v>-17.712630000000001</v>
+      </c>
+      <c r="V46">
+        <f>EXP(R46)</f>
+        <v>5.3614563805160336E-7</v>
+      </c>
+      <c r="W46">
+        <f t="shared" ref="W46:X47" si="28">EXP(S46)</f>
+        <v>1.0028296468727901E-7</v>
+      </c>
+      <c r="X46">
+        <f t="shared" si="28"/>
+        <v>2.0300303505511811E-8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" ht="24" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>95</v>
       </c>
       <c r="B47" s="1">
         <v>1</v>
       </c>
       <c r="C47">
+        <f t="shared" si="25"/>
+        <v>110</v>
+      </c>
+      <c r="D47">
         <f t="shared" si="24"/>
-        <v>110</v>
-      </c>
-      <c r="D47">
-        <f t="shared" si="23"/>
         <v>55</v>
       </c>
       <c r="E47" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>181</v>
       </c>
       <c r="F47">
@@ -2707,29 +3409,73 @@
       <c r="H47">
         <v>185</v>
       </c>
+      <c r="I47">
+        <f t="shared" si="7"/>
+        <v>1.81E-10</v>
+      </c>
       <c r="J47" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>5.1984970312658261</v>
       </c>
-    </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K47" s="3">
+        <f t="shared" si="4"/>
+        <v>-22.432524084662724</v>
+      </c>
+      <c r="M47" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N47" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="O47" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="P47" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q47" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="R47">
+        <v>-9.6077100000000009</v>
+      </c>
+      <c r="S47">
+        <v>-9.2610200000000003</v>
+      </c>
+      <c r="T47">
+        <v>-9.6968700000000005</v>
+      </c>
+      <c r="V47">
+        <f>EXP(R47)</f>
+        <v>6.7208555805853515E-5</v>
+      </c>
+      <c r="W47">
+        <f t="shared" si="28"/>
+        <v>9.5058316196068538E-5</v>
+      </c>
+      <c r="X47">
+        <f t="shared" si="28"/>
+        <v>6.1475612900322769E-5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" ht="24" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>97</v>
       </c>
       <c r="B48" s="1">
         <v>0.8</v>
       </c>
       <c r="C48">
+        <f t="shared" si="25"/>
+        <v>88</v>
+      </c>
+      <c r="D48">
         <f t="shared" si="24"/>
-        <v>88</v>
-      </c>
-      <c r="D48">
-        <f t="shared" si="23"/>
         <v>44</v>
       </c>
       <c r="E48" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>116</v>
       </c>
       <c r="F48">
@@ -2741,29 +3487,76 @@
       <c r="H48">
         <v>112</v>
       </c>
+      <c r="I48">
+        <f t="shared" si="7"/>
+        <v>1.16E-10</v>
+      </c>
       <c r="J48" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>4.7535901911063645</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K48" s="3">
+        <f t="shared" si="4"/>
+        <v>-22.877430924822182</v>
+      </c>
+      <c r="M48" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="N48" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="O48" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="P48" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q48" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="R48">
+        <v>-4.0106799999999998</v>
+      </c>
+      <c r="S48">
+        <v>-2.4928900000000001</v>
+      </c>
+      <c r="T48">
+        <v>-1.5214099999999999</v>
+      </c>
+      <c r="U48" t="s">
+        <v>77</v>
+      </c>
+      <c r="V48">
+        <f>EXP(1/R48)</f>
+        <v>0.77931942090725548</v>
+      </c>
+      <c r="W48">
+        <f t="shared" ref="W48:X48" si="29">EXP(1/S48)</f>
+        <v>0.66955575111011467</v>
+      </c>
+      <c r="X48">
+        <f t="shared" si="29"/>
+        <v>0.51825648291462234</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" ht="24" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>99</v>
       </c>
       <c r="B49" s="1">
         <v>0.6</v>
       </c>
       <c r="C49">
+        <f t="shared" si="25"/>
+        <v>66</v>
+      </c>
+      <c r="D49">
         <f t="shared" si="24"/>
-        <v>66</v>
-      </c>
-      <c r="D49">
-        <f t="shared" si="23"/>
         <v>33</v>
       </c>
       <c r="E49" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>66.666666666666671</v>
       </c>
       <c r="F49">
@@ -2775,29 +3568,49 @@
       <c r="H49">
         <v>65</v>
       </c>
+      <c r="I49">
+        <f t="shared" si="7"/>
+        <v>6.6666666666666669E-11</v>
+      </c>
       <c r="J49" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>4.1997050778799272</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K49" s="3">
+        <f t="shared" si="4"/>
+        <v>-23.431316038048621</v>
+      </c>
+      <c r="M49" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="N49" s="9">
+        <v>2.1800000000000001E-3</v>
+      </c>
+      <c r="O49" s="21">
+        <v>8.2982100000000001E-4</v>
+      </c>
+      <c r="P49" s="10">
+        <v>3.3579999999999999E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" ht="24" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>101</v>
       </c>
       <c r="B50" s="1">
         <v>0.4</v>
       </c>
       <c r="C50">
+        <f t="shared" si="25"/>
+        <v>44</v>
+      </c>
+      <c r="D50">
         <f t="shared" si="24"/>
-        <v>44</v>
-      </c>
-      <c r="D50">
-        <f t="shared" si="23"/>
         <v>22</v>
       </c>
       <c r="E50" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>35.666666666666664</v>
       </c>
       <c r="F50">
@@ -2809,29 +3622,49 @@
       <c r="H50">
         <v>38</v>
       </c>
+      <c r="I50">
+        <f t="shared" si="7"/>
+        <v>3.5666666666666666E-11</v>
+      </c>
       <c r="J50" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>3.5742165457937962</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K50" s="3">
+        <f t="shared" si="4"/>
+        <v>-24.056804570134751</v>
+      </c>
+      <c r="M50" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="N50" s="9">
+        <v>0.99922</v>
+      </c>
+      <c r="O50" s="9">
+        <v>0.99948000000000004</v>
+      </c>
+      <c r="P50" s="10">
+        <v>0.99338000000000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>103</v>
       </c>
       <c r="B51" s="1">
         <v>0.2</v>
       </c>
       <c r="C51">
+        <f t="shared" si="25"/>
+        <v>22</v>
+      </c>
+      <c r="D51">
         <f t="shared" si="24"/>
-        <v>22</v>
-      </c>
-      <c r="D51">
-        <f t="shared" si="23"/>
         <v>11</v>
       </c>
       <c r="E51" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>14.666666666666666</v>
       </c>
       <c r="F51">
@@ -2843,12 +3676,47 @@
       <c r="H51">
         <v>15</v>
       </c>
+      <c r="I51">
+        <f t="shared" si="7"/>
+        <v>1.4666666666666664E-11</v>
+      </c>
       <c r="J51" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>2.6855773452501515</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K51" s="3">
+        <f t="shared" si="4"/>
+        <v>-24.945443770678398</v>
+      </c>
+      <c r="M51" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N51" s="12">
+        <v>0.999</v>
+      </c>
+      <c r="O51" s="12">
+        <v>0.99933000000000005</v>
+      </c>
+      <c r="P51" s="13">
+        <v>0.99148999999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M52" s="3"/>
+      <c r="T52">
+        <v>90</v>
+      </c>
+      <c r="U52">
+        <v>110</v>
+      </c>
+      <c r="W52">
+        <v>90</v>
+      </c>
+      <c r="X52">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>0</v>
       </c>
@@ -2858,8 +3726,38 @@
       <c r="D53" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M53" s="3"/>
+      <c r="N53" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="O53" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="P53" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q53" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="S53" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="T53">
+        <v>-16.756959999999999</v>
+      </c>
+      <c r="U53">
+        <v>-14.63026</v>
+      </c>
+      <c r="W53">
+        <f>EXP(T53)</f>
+        <v>5.278915843438181E-8</v>
+      </c>
+      <c r="X53">
+        <f>EXP(U53)</f>
+        <v>4.4275024806557514E-7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" ht="36" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -2875,8 +3773,37 @@
       <c r="E54" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N54" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="O54" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="P54" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q54" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="S54" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="T54">
+        <v>-7.9023300000000001</v>
+      </c>
+      <c r="U54">
+        <v>-10.922510000000001</v>
+      </c>
+      <c r="W54">
+        <f>EXP(T54)</f>
+        <v>3.6988071359346714E-4</v>
+      </c>
+      <c r="X54">
+        <f>EXP(U54)</f>
+        <v>1.804738065106965E-5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" ht="24" x14ac:dyDescent="0.25">
       <c r="A55">
         <f>85</f>
         <v>85</v>
@@ -2889,11 +3816,11 @@
         <v>240</v>
       </c>
       <c r="D55">
-        <f t="shared" ref="D55:D64" si="27">C55/2</f>
+        <f t="shared" ref="D55:D64" si="30">C55/2</f>
         <v>120</v>
       </c>
       <c r="E55" s="2">
-        <f t="shared" ref="E55:E64" si="28">AVERAGE(F55,G55,H55)</f>
+        <f t="shared" ref="E55:E64" si="31">AVERAGE(F55,G55,H55)</f>
         <v>1862.3333333333333</v>
       </c>
       <c r="F55">
@@ -2905,12 +3832,52 @@
       <c r="H55">
         <v>1858</v>
       </c>
+      <c r="I55">
+        <f t="shared" si="7"/>
+        <v>1.8623333333333332E-9</v>
+      </c>
       <c r="J55" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>7.5295854607910391</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K55" s="3">
+        <f t="shared" si="4"/>
+        <v>-20.101435655137511</v>
+      </c>
+      <c r="N55" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="O55" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="P55" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q55" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S55" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="T55">
+        <v>-2.3885200000000002</v>
+      </c>
+      <c r="U55">
+        <v>-2.9170400000000001</v>
+      </c>
+      <c r="V55" t="s">
+        <v>77</v>
+      </c>
+      <c r="W55">
+        <f>EXP(1/T55)</f>
+        <v>0.65792173303153134</v>
+      </c>
+      <c r="X55">
+        <f>EXP(1/U55)</f>
+        <v>0.70977073981517713</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" ht="24" x14ac:dyDescent="0.25">
       <c r="A56">
         <f>A55+2</f>
         <v>87</v>
@@ -2919,15 +3886,15 @@
         <v>1.8</v>
       </c>
       <c r="C56">
-        <f t="shared" ref="C56:C64" si="29">C$53*$B56</f>
+        <f t="shared" ref="C56:C64" si="32">C$53*$B56</f>
         <v>216</v>
       </c>
       <c r="D56">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>108</v>
       </c>
       <c r="E56" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>1043.6666666666667</v>
       </c>
       <c r="F56">
@@ -2939,29 +3906,49 @@
       <c r="H56">
         <v>1045</v>
       </c>
+      <c r="I56">
+        <f t="shared" si="7"/>
+        <v>1.0436666666666667E-9</v>
+      </c>
       <c r="J56" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>6.9504954326582959</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K56" s="3">
+        <f t="shared" si="4"/>
+        <v>-20.68052568327025</v>
+      </c>
+      <c r="N56" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="O56" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="P56" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q56" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" ht="24" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" ref="A57:A64" si="30">A56+2</f>
+        <f t="shared" ref="A57:A64" si="33">A56+2</f>
         <v>89</v>
       </c>
       <c r="B57" s="1">
         <v>1.6</v>
       </c>
       <c r="C57">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>192</v>
       </c>
       <c r="D57">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>96</v>
       </c>
       <c r="E57" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>598.66666666666663</v>
       </c>
       <c r="F57">
@@ -2973,29 +3960,49 @@
       <c r="H57">
         <v>600</v>
       </c>
+      <c r="I57">
+        <f t="shared" si="7"/>
+        <v>5.9866666666666667E-10</v>
+      </c>
       <c r="J57" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>6.3947049601940353</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K57" s="3">
+        <f t="shared" si="4"/>
+        <v>-21.236316155734514</v>
+      </c>
+      <c r="N57" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O57" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="P57" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q57" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" ht="24" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>91</v>
       </c>
       <c r="B58" s="1">
         <v>1.4</v>
       </c>
       <c r="C58">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>168</v>
       </c>
       <c r="D58">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>84</v>
       </c>
       <c r="E58" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>353.66666666666669</v>
       </c>
       <c r="F58">
@@ -3007,29 +4014,49 @@
       <c r="H58">
         <v>352</v>
       </c>
+      <c r="I58">
+        <f t="shared" si="7"/>
+        <v>3.5366666666666669E-10</v>
+      </c>
       <c r="J58" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>5.8683548499458738</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K58" s="3">
+        <f t="shared" si="4"/>
+        <v>-21.762666265982674</v>
+      </c>
+      <c r="N58" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="O58" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="P58" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q58" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" ht="24" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>93</v>
       </c>
       <c r="B59" s="1">
         <v>1.2</v>
       </c>
       <c r="C59">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>144</v>
       </c>
       <c r="D59">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>72</v>
       </c>
       <c r="E59" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>224.66666666666666</v>
       </c>
       <c r="F59">
@@ -3041,29 +4068,49 @@
       <c r="H59">
         <v>223</v>
       </c>
+      <c r="I59">
+        <f t="shared" si="7"/>
+        <v>2.2466666666666667E-10</v>
+      </c>
       <c r="J59" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>5.414617822244197</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K59" s="3">
+        <f t="shared" si="4"/>
+        <v>-22.216403293684351</v>
+      </c>
+      <c r="N59" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O59" s="10">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="P59" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q59" s="10">
+        <v>6.8700000000000002E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" ht="24" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>95</v>
       </c>
       <c r="B60" s="1">
         <v>1</v>
       </c>
       <c r="C60">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>120</v>
       </c>
       <c r="D60">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>60</v>
       </c>
       <c r="E60" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>125</v>
       </c>
       <c r="F60">
@@ -3075,29 +4122,49 @@
       <c r="H60">
         <v>122</v>
       </c>
+      <c r="I60">
+        <f t="shared" si="7"/>
+        <v>1.2500000000000001E-10</v>
+      </c>
       <c r="J60" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>4.8283137373023015</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K60" s="3">
+        <f t="shared" si="4"/>
+        <v>-22.802707378626248</v>
+      </c>
+      <c r="N60" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="O60" s="10">
+        <v>0.99804999999999999</v>
+      </c>
+      <c r="P60" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q60" s="10">
+        <v>0.99785999999999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" ht="24" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>97</v>
       </c>
       <c r="B61" s="1">
         <v>0.8</v>
       </c>
       <c r="C61">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>96</v>
       </c>
       <c r="D61">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>48</v>
       </c>
       <c r="E61" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>76.333333333333329</v>
       </c>
       <c r="F61">
@@ -3109,29 +4176,49 @@
       <c r="H61">
         <v>82</v>
       </c>
+      <c r="I61">
+        <f t="shared" si="7"/>
+        <v>7.6333333333333328E-11</v>
+      </c>
       <c r="J61" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>4.33510971488613</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K61" s="3">
+        <f t="shared" si="4"/>
+        <v>-23.295911401042417</v>
+      </c>
+      <c r="N61" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="O61" s="13">
+        <v>0.99748999999999999</v>
+      </c>
+      <c r="P61" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q61" s="13">
+        <v>0.99724999999999997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>99</v>
       </c>
       <c r="B62" s="1">
         <v>0.6</v>
       </c>
       <c r="C62">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>72</v>
       </c>
       <c r="D62">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>36</v>
       </c>
       <c r="E62" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>34.333333333333336</v>
       </c>
       <c r="F62">
@@ -3143,29 +4230,37 @@
       <c r="H62">
         <v>34</v>
       </c>
+      <c r="I62">
+        <f t="shared" si="7"/>
+        <v>3.4333333333333338E-11</v>
+      </c>
       <c r="J62" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>3.5361166995615263</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K62" s="3">
+        <f t="shared" si="4"/>
+        <v>-24.094904416367022</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>101</v>
       </c>
       <c r="B63" s="1">
         <v>0.4</v>
       </c>
       <c r="C63">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>48</v>
       </c>
       <c r="D63">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>24</v>
       </c>
       <c r="E63" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>14</v>
       </c>
       <c r="F63">
@@ -3177,29 +4272,37 @@
       <c r="H63">
         <v>16</v>
       </c>
+      <c r="I63">
+        <f t="shared" si="7"/>
+        <v>1.4E-11</v>
+      </c>
       <c r="J63" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>2.6390573296152584</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K63" s="3">
+        <f t="shared" si="4"/>
+        <v>-24.991963786313288</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>103</v>
       </c>
       <c r="B64" s="1">
         <v>0.2</v>
       </c>
       <c r="C64">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>24</v>
       </c>
       <c r="D64">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="E64" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="F64">
@@ -3211,12 +4314,24 @@
       <c r="H64">
         <v>4</v>
       </c>
+      <c r="I64">
+        <f t="shared" si="7"/>
+        <v>3.3333333333333335E-12</v>
+      </c>
       <c r="J64" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1.2039728043259361</v>
       </c>
+      <c r="K64" s="3">
+        <f t="shared" si="4"/>
+        <v>-26.427048311602611</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="N43:P43"/>
+    <mergeCell ref="N44:P44"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
01: Add iposun as demanded In progress
</commit_message>
<xml_diff>
--- a/01_Townsend/data/Townsend.xlsx
+++ b/01_Townsend/data/Townsend.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\Škola Mgr\Praktikum plazma\PraktikaPlazma\01_Townsend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A7D2FB-B895-4B68-84F8-84FC102BFE77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D0A2E6-ECBD-4438-A2EC-F7C477A16C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="84">
   <si>
     <t>Vcm-1</t>
   </si>
@@ -180,51 +180,9 @@
     <t>Model</t>
   </si>
   <si>
-    <t>ExpGro1</t>
-  </si>
-  <si>
-    <t>y = A1*exp(x/t1) + y0</t>
-  </si>
-  <si>
-    <t>y0</t>
-  </si>
-  <si>
-    <t>-17,71263 ± 0,96317</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>-9,69687 ± 0,78472</t>
-  </si>
-  <si>
-    <t>t1</t>
-  </si>
-  <si>
-    <t>-1,52141 ± 0,29447</t>
-  </si>
-  <si>
     <t>Reduced Chi-Sqr</t>
   </si>
   <si>
-    <t>-14,43886 ± 1,01438</t>
-  </si>
-  <si>
-    <t>-16,11527 ± 0,64138</t>
-  </si>
-  <si>
-    <t>-9,60771 ± 0,98565</t>
-  </si>
-  <si>
-    <t>-9,26102 ± 0,5943</t>
-  </si>
-  <si>
-    <t>-4,01068 ± 0,5527</t>
-  </si>
-  <si>
-    <t>-2,49289 ± 0,26295</t>
-  </si>
-  <si>
     <t>100 Vcm\+(-1)</t>
   </si>
   <si>
@@ -234,40 +192,100 @@
     <t>120 Vcm\+(-1)</t>
   </si>
   <si>
-    <t>I posun</t>
-  </si>
-  <si>
-    <t>1/alpha</t>
-  </si>
-  <si>
-    <t>I0</t>
-  </si>
-  <si>
     <t>90 Vcm\+(-1)</t>
   </si>
   <si>
-    <t>-16,75696 ± 0,81858</t>
-  </si>
-  <si>
-    <t>-7,90233 ± 0,75321</t>
-  </si>
-  <si>
-    <t>-2,38852 ± 0,38346</t>
-  </si>
-  <si>
     <t>110 Vcm\+(-1)</t>
   </si>
   <si>
-    <t>-14,63026 ± 1,55229</t>
-  </si>
-  <si>
-    <t>-10,92251 ± 1,46892</t>
-  </si>
-  <si>
-    <t>-2,91704 ± 0,59548</t>
-  </si>
-  <si>
     <t>alpha</t>
+  </si>
+  <si>
+    <t>i posun</t>
+  </si>
+  <si>
+    <t>lnposun (User)</t>
+  </si>
+  <si>
+    <t>ln(i0*exp(A*x)+ip)</t>
+  </si>
+  <si>
+    <t>1,60012 ± 0,05494</t>
+  </si>
+  <si>
+    <t>2,03335 ± 0,03657</t>
+  </si>
+  <si>
+    <t>2,57037 ± 0,05346</t>
+  </si>
+  <si>
+    <t>6,73919E-11 ± 6,3373E-12</t>
+  </si>
+  <si>
+    <t>2,94773E-11 ± 1,67729E-12</t>
+  </si>
+  <si>
+    <t>1,05525E-11 ± 8,07335E-13</t>
+  </si>
+  <si>
+    <t>ip</t>
+  </si>
+  <si>
+    <t>-3,61428E-11 ± 8,9411E-12</t>
+  </si>
+  <si>
+    <t>-2,60703E-11 ± 2,48659E-12</t>
+  </si>
+  <si>
+    <t>-1,43552E-11 ± 1,22151E-12</t>
+  </si>
+  <si>
+    <t>1,69129 ± 0,0273</t>
+  </si>
+  <si>
+    <t>2,21671 ± 0,02584</t>
+  </si>
+  <si>
+    <t>6,34609E-11 ± 2,83291E-12</t>
+  </si>
+  <si>
+    <t>2,28835E-11 ± 9,01119E-13</t>
+  </si>
+  <si>
+    <t>-5,49481E-11 ± 3,8619E-12</t>
+  </si>
+  <si>
+    <t>-2,07998E-11 ± 1,39314E-12</t>
+  </si>
+  <si>
+    <t>y = a + b*x</t>
+  </si>
+  <si>
+    <t>ln α/p</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>No Weighting</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>2,09311 ± 0,1572</t>
+  </si>
+  <si>
+    <t>Slope</t>
+  </si>
+  <si>
+    <t>-0,14475 ± 0,01917</t>
+  </si>
+  <si>
+    <t>Residual Sum of Squares</t>
+  </si>
+  <si>
+    <t>Pearson's r</t>
   </si>
 </sst>
 </file>
@@ -328,7 +346,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -495,11 +513,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -528,10 +564,19 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -546,15 +591,27 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -893,27 +950,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA64"/>
+  <dimension ref="A1:AE90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="S58" sqref="S58"/>
+    <sheetView tabSelected="1" topLeftCell="G70" workbookViewId="0">
+      <selection activeCell="X90" sqref="X90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" style="3"/>
-    <col min="12" max="12" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="3"/>
+    <col min="11" max="11" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" customWidth="1"/>
     <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" customWidth="1"/>
-    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.140625" customWidth="1"/>
-    <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.85546875" customWidth="1"/>
+    <col min="24" max="24" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.140625" customWidth="1"/>
+    <col min="29" max="29" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
@@ -926,15 +991,15 @@
       <c r="K1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="3">
+      <c r="M1" s="3">
         <f>50*1.59</f>
         <v>79.5</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -959,29 +1024,31 @@
       <c r="K2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="1"/>
+      <c r="O2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" s="3"/>
+      <c r="Q2" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="T2" t="s">
+      <c r="X2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>85</f>
         <v>85</v>
@@ -1022,14 +1089,14 @@
         <f>LN(I3)</f>
         <v>-20.222086590232227</v>
       </c>
-      <c r="L3" s="3">
+      <c r="M3" s="3">
         <v>80</v>
       </c>
-      <c r="T3" t="s">
+      <c r="X3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+2</f>
         <v>87</v>
@@ -1070,14 +1137,14 @@
         <f t="shared" ref="K4:K64" si="4">LN(I4)</f>
         <v>-20.61800532628892</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <v>90</v>
       </c>
-      <c r="S4" t="s">
+      <c r="W4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:A12" si="5">A4+2</f>
         <v>89</v>
@@ -1118,14 +1185,14 @@
         <f t="shared" si="4"/>
         <v>-21.009171709996938</v>
       </c>
-      <c r="L5" s="3">
+      <c r="M5" s="3">
         <v>100</v>
       </c>
-      <c r="T5" t="s">
+      <c r="X5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="5"/>
         <v>91</v>
@@ -1166,14 +1233,14 @@
         <f t="shared" si="4"/>
         <v>-21.451694831650997</v>
       </c>
-      <c r="L6" s="3">
+      <c r="M6" s="3">
         <v>110</v>
       </c>
-      <c r="T6" t="s">
+      <c r="X6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="5"/>
         <v>93</v>
@@ -1214,14 +1281,14 @@
         <f t="shared" si="4"/>
         <v>-21.848222100954121</v>
       </c>
-      <c r="L7" s="3">
+      <c r="M7" s="3">
         <v>120</v>
       </c>
-      <c r="S7" t="s">
+      <c r="W7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="5"/>
         <v>95</v>
@@ -1262,11 +1329,11 @@
         <f t="shared" si="4"/>
         <v>-22.346126769712651</v>
       </c>
-      <c r="T8" t="s">
+      <c r="X8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="5"/>
         <v>97</v>
@@ -1307,14 +1374,15 @@
         <f t="shared" si="4"/>
         <v>-22.792097199514231</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="M9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="T9" s="5" t="s">
+      <c r="N9" s="4"/>
+      <c r="X9" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="5"/>
         <v>99</v>
@@ -1355,47 +1423,49 @@
         <f t="shared" si="4"/>
         <v>-23.322461633136538</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="N10" s="1"/>
+      <c r="O10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="N10" t="s">
+      <c r="P10" s="3"/>
+      <c r="Q10" t="s">
         <v>23</v>
       </c>
-      <c r="O10" t="s">
+      <c r="S10" t="s">
         <v>19</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="T10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q10" s="3" t="s">
+      <c r="U10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R10" s="3" t="s">
+      <c r="V10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="X10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U10" s="3" t="s">
+      <c r="Y10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="W10" t="s">
+      <c r="AA10" t="s">
         <v>19</v>
       </c>
-      <c r="X10" s="3" t="s">
+      <c r="AB10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Y10" s="3" t="s">
+      <c r="AC10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Z10" s="3" t="s">
+      <c r="AD10" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="5"/>
         <v>101</v>
@@ -1436,30 +1506,30 @@
         <f t="shared" si="4"/>
         <v>-24.002245585884317</v>
       </c>
-      <c r="L11" s="3">
+      <c r="M11" s="3">
         <v>80</v>
       </c>
-      <c r="M11">
+      <c r="O11">
         <v>1.8319300000000001</v>
       </c>
-      <c r="N11">
+      <c r="Q11">
         <v>3.7988</v>
       </c>
-      <c r="Q11">
-        <f>EXP(N11)</f>
+      <c r="U11">
+        <f t="shared" ref="U11:U20" si="8">EXP(Q11)</f>
         <v>44.647575243891616</v>
       </c>
-      <c r="T11" s="3">
+      <c r="X11" s="3">
         <v>80</v>
       </c>
-      <c r="U11">
+      <c r="Y11">
         <v>1.6020799999999999</v>
       </c>
-      <c r="Y11">
+      <c r="AC11">
         <v>63.650860000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="5"/>
         <v>103</v>
@@ -1500,54 +1570,54 @@
         <f t="shared" si="4"/>
         <v>-24.704281713861509</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="M12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M12">
+      <c r="O12">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="N12">
+      <c r="Q12">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="Q12">
-        <f>EXP(N12)</f>
+      <c r="U12">
+        <f t="shared" si="8"/>
         <v>1.0554846021550801</v>
       </c>
-      <c r="T12" s="3" t="s">
+      <c r="X12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U12">
+      <c r="Y12">
         <v>5.722E-2</v>
       </c>
-      <c r="Y12">
+      <c r="AC12">
         <v>6.6234200000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="L13" s="3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="M13" s="3">
         <v>90</v>
       </c>
-      <c r="M13">
+      <c r="O13">
         <v>2.1239699999999999</v>
       </c>
-      <c r="N13">
+      <c r="Q13">
         <v>3.4063099999999999</v>
       </c>
-      <c r="Q13">
-        <f>EXP(N13)</f>
+      <c r="U13">
+        <f t="shared" si="8"/>
         <v>30.153771302174523</v>
       </c>
-      <c r="T13" s="3">
+      <c r="X13" s="3">
         <v>90</v>
       </c>
-      <c r="U13">
+      <c r="Y13">
         <v>1.8524799999999999</v>
       </c>
-      <c r="Y13">
+      <c r="AC13">
         <v>45.298009999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1557,30 +1627,30 @@
       <c r="D14" t="s">
         <v>4</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="M14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M14">
+      <c r="O14">
         <v>8.4290000000000004E-2</v>
       </c>
-      <c r="N14">
+      <c r="Q14">
         <v>0.1046</v>
       </c>
-      <c r="Q14">
-        <f>EXP(N14)</f>
+      <c r="U14">
+        <f t="shared" si="8"/>
         <v>1.1102664149565653</v>
       </c>
-      <c r="T14" s="3" t="s">
+      <c r="X14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U14">
+      <c r="Y14">
         <v>3.3259999999999998E-2</v>
       </c>
-      <c r="Y14">
+      <c r="AC14">
         <v>2.79297</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1596,30 +1666,30 @@
       <c r="E15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L15" s="3">
+      <c r="M15" s="3">
         <v>100</v>
       </c>
-      <c r="M15">
+      <c r="O15">
         <v>2.4277299999999999</v>
       </c>
-      <c r="N15">
+      <c r="Q15">
         <v>2.7288800000000002</v>
       </c>
-      <c r="Q15">
-        <f>EXP(N15)</f>
+      <c r="U15">
+        <f t="shared" si="8"/>
         <v>15.315723799642379</v>
       </c>
-      <c r="T15" s="3">
+      <c r="X15" s="3">
         <v>100</v>
       </c>
-      <c r="U15">
+      <c r="Y15">
         <v>2.0671499999999998</v>
       </c>
-      <c r="Y15">
+      <c r="AC15">
         <v>26.650030000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>85</f>
         <v>85</v>
@@ -1632,7 +1702,7 @@
         <v>160</v>
       </c>
       <c r="D16">
-        <f t="shared" ref="D16:D25" si="8">C16/2</f>
+        <f t="shared" ref="D16:D25" si="9">C16/2</f>
         <v>80</v>
       </c>
       <c r="E16" s="2">
@@ -1660,30 +1730,30 @@
         <f t="shared" si="4"/>
         <v>-20.308290538837255</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M16">
+      <c r="O16">
         <v>8.8819999999999996E-2</v>
       </c>
-      <c r="N16">
+      <c r="Q16">
         <v>0.11022</v>
       </c>
-      <c r="Q16">
-        <f>EXP(N16)</f>
+      <c r="U16">
+        <f t="shared" si="8"/>
         <v>1.1165236786502826</v>
       </c>
-      <c r="T16" s="3" t="s">
+      <c r="X16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U16">
+      <c r="Y16">
         <v>3.3950000000000001E-2</v>
       </c>
-      <c r="Y16">
+      <c r="AC16">
         <v>1.6993199999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>A16+2</f>
         <v>87</v>
@@ -1692,15 +1762,15 @@
         <v>1.8</v>
       </c>
       <c r="C17">
-        <f t="shared" ref="C17:C25" si="9">C$14*$B17</f>
+        <f t="shared" ref="C17:C25" si="10">C$14*$B17</f>
         <v>144</v>
       </c>
       <c r="D17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>72</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" ref="E17:E25" si="10">AVERAGE(F17,G17,H17)</f>
+        <f t="shared" ref="E17:E25" si="11">AVERAGE(F17,G17,H17)</f>
         <v>1201.6666666666667</v>
       </c>
       <c r="F17">
@@ -1724,47 +1794,47 @@
         <f t="shared" si="4"/>
         <v>-20.539556354877607</v>
       </c>
-      <c r="L17" s="3">
+      <c r="M17" s="3">
         <v>110</v>
       </c>
-      <c r="M17">
+      <c r="O17">
         <v>2.5981700000000001</v>
       </c>
-      <c r="N17">
+      <c r="Q17">
         <v>2.5054599999999998</v>
       </c>
-      <c r="Q17">
-        <f>EXP(N17)</f>
+      <c r="U17">
+        <f t="shared" si="8"/>
         <v>12.249192298492478</v>
       </c>
-      <c r="T17" s="3">
+      <c r="X17" s="3">
         <v>110</v>
       </c>
-      <c r="U17">
+      <c r="Y17">
         <v>2.2840400000000001</v>
       </c>
-      <c r="Y17">
+      <c r="AC17">
         <v>19.918209999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" ref="A18:A25" si="11">A17+2</f>
+        <f t="shared" ref="A18:A25" si="12">A17+2</f>
         <v>89</v>
       </c>
       <c r="B18" s="1">
         <v>1.6</v>
       </c>
       <c r="C18">
+        <f t="shared" si="10"/>
+        <v>128</v>
+      </c>
+      <c r="D18">
         <f t="shared" si="9"/>
-        <v>128</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="8"/>
         <v>64</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>853</v>
       </c>
       <c r="F18">
@@ -1788,47 +1858,47 @@
         <f t="shared" si="4"/>
         <v>-20.882261568436871</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="M18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M18">
+      <c r="O18">
         <v>8.8469999999999993E-2</v>
       </c>
-      <c r="N18">
+      <c r="Q18">
         <v>0.10979</v>
       </c>
-      <c r="Q18">
-        <f>EXP(N18)</f>
+      <c r="U18">
+        <f t="shared" si="8"/>
         <v>1.1160436766762836</v>
       </c>
-      <c r="T18" s="3" t="s">
+      <c r="X18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U18">
+      <c r="Y18">
         <v>3.2439999999999997E-2</v>
       </c>
-      <c r="Y18">
+      <c r="AC18">
         <v>1.22679</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>91</v>
       </c>
       <c r="B19" s="1">
         <v>1.4</v>
       </c>
       <c r="C19">
+        <f t="shared" si="10"/>
+        <v>112</v>
+      </c>
+      <c r="D19">
         <f t="shared" si="9"/>
-        <v>112</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="8"/>
         <v>56</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>622</v>
       </c>
       <c r="F19">
@@ -1852,47 +1922,47 @@
         <f t="shared" si="4"/>
         <v>-21.198081023189367</v>
       </c>
-      <c r="L19" s="3">
+      <c r="M19" s="3">
         <v>120</v>
       </c>
-      <c r="M19">
+      <c r="O19">
         <v>2.91371</v>
       </c>
-      <c r="N19">
+      <c r="Q19">
         <v>1.7809200000000001</v>
       </c>
-      <c r="Q19">
-        <f>EXP(N19)</f>
+      <c r="U19">
+        <f t="shared" si="8"/>
         <v>5.9353143967812478</v>
       </c>
-      <c r="T19" s="3">
+      <c r="X19" s="3">
         <v>120</v>
       </c>
-      <c r="U19">
+      <c r="Y19">
         <v>2.7817500000000002</v>
       </c>
-      <c r="Y19">
+      <c r="AC19">
         <v>7.1057199999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>93</v>
       </c>
       <c r="B20" s="1">
         <v>1.2</v>
       </c>
       <c r="C20">
+        <f t="shared" si="10"/>
+        <v>96</v>
+      </c>
+      <c r="D20">
         <f t="shared" si="9"/>
-        <v>96</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="8"/>
         <v>48</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>435.33333333333331</v>
       </c>
       <c r="F20">
@@ -1916,47 +1986,47 @@
         <f t="shared" si="4"/>
         <v>-21.55490909476028</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="M20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M20">
+      <c r="O20">
         <v>0.10781</v>
       </c>
-      <c r="N20">
+      <c r="Q20">
         <v>0.14085</v>
       </c>
-      <c r="Q20">
-        <f>EXP(N20)</f>
+      <c r="U20">
+        <f t="shared" si="8"/>
         <v>1.1512519472404261</v>
       </c>
-      <c r="T20" s="3" t="s">
+      <c r="X20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U20">
+      <c r="Y20">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="Y20">
+      <c r="AC20">
         <v>0.501</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>95</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
       </c>
       <c r="C21">
+        <f t="shared" si="10"/>
+        <v>80</v>
+      </c>
+      <c r="D21">
         <f t="shared" si="9"/>
-        <v>80</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="8"/>
         <v>40</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>300.66666666666669</v>
       </c>
       <c r="F21">
@@ -1980,26 +2050,26 @@
         <f t="shared" si="4"/>
         <v>-21.925018884534033</v>
       </c>
-      <c r="T21" s="3"/>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X21" s="3"/>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>97</v>
       </c>
       <c r="B22" s="1">
         <v>0.8</v>
       </c>
       <c r="C22">
+        <f t="shared" si="10"/>
+        <v>64</v>
+      </c>
+      <c r="D22">
         <f t="shared" si="9"/>
-        <v>64</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="8"/>
         <v>32</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>196</v>
       </c>
       <c r="F22">
@@ -2023,55 +2093,57 @@
         <f t="shared" si="4"/>
         <v>-22.35290645669803</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="M22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M22" s="3" t="s">
+      <c r="N22" s="1"/>
+      <c r="O22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="N22" t="s">
+      <c r="P22" s="3"/>
+      <c r="Q22" t="s">
         <v>28</v>
       </c>
-      <c r="O22" s="3" t="s">
+      <c r="S22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P22" s="3" t="s">
+      <c r="T22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="T22" s="1" t="s">
+      <c r="X22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U22" s="3" t="s">
+      <c r="Y22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="V22" t="s">
+      <c r="Z22" t="s">
         <v>28</v>
       </c>
-      <c r="W22" s="3" t="s">
+      <c r="AA22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="X22" s="3" t="s">
+      <c r="AB22" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>99</v>
       </c>
       <c r="B23" s="1">
         <v>0.6</v>
       </c>
       <c r="C23">
+        <f t="shared" si="10"/>
+        <v>48</v>
+      </c>
+      <c r="D23">
         <f t="shared" si="9"/>
-        <v>48</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="8"/>
         <v>24</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>135</v>
       </c>
       <c r="F23">
@@ -2095,71 +2167,71 @@
         <f t="shared" si="4"/>
         <v>-22.725746337490119</v>
       </c>
-      <c r="L23" s="3">
+      <c r="M23" s="3">
         <v>8000</v>
       </c>
-      <c r="M23">
-        <f>M11*100</f>
+      <c r="O23">
+        <f>O11*100</f>
         <v>183.19300000000001</v>
       </c>
-      <c r="N23">
-        <f>M23/$L$1</f>
+      <c r="Q23">
+        <f>O23/$M$1</f>
         <v>2.304314465408805</v>
       </c>
-      <c r="O23">
-        <f>LN(N23)</f>
+      <c r="S23">
+        <f>LN(Q23)</f>
         <v>0.8347832202427512</v>
       </c>
-      <c r="P23">
-        <f>$L$1/L23</f>
+      <c r="T23">
+        <f>$M$1/M23</f>
         <v>9.9375000000000002E-3</v>
       </c>
-      <c r="Q23">
-        <f>P23*1000</f>
+      <c r="U23">
+        <f>T23*1000</f>
         <v>9.9375</v>
       </c>
-      <c r="T23" s="3">
+      <c r="X23" s="3">
         <v>8000</v>
       </c>
-      <c r="U23">
-        <f>U11*100</f>
+      <c r="Y23">
+        <f>Y11*100</f>
         <v>160.208</v>
       </c>
-      <c r="V23">
-        <f>U23/$L$1</f>
+      <c r="Z23">
+        <f>Y23/$M$1</f>
         <v>2.0151949685534589</v>
       </c>
-      <c r="W23">
-        <f>LN(V23)</f>
+      <c r="AA23">
+        <f>LN(Z23)</f>
         <v>0.70071594930516068</v>
       </c>
-      <c r="X23">
-        <f>$L$1/T23</f>
+      <c r="AB23">
+        <f>$M$1/X23</f>
         <v>9.9375000000000002E-3</v>
       </c>
-      <c r="Y23">
-        <f>X23*1000</f>
+      <c r="AC23">
+        <f>AB23*1000</f>
         <v>9.9375</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>101</v>
       </c>
       <c r="B24" s="1">
         <v>0.4</v>
       </c>
       <c r="C24">
+        <f t="shared" si="10"/>
+        <v>32</v>
+      </c>
+      <c r="D24">
         <f t="shared" si="9"/>
-        <v>32</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>92.666666666666671</v>
       </c>
       <c r="F24">
@@ -2183,71 +2255,71 @@
         <f t="shared" si="4"/>
         <v>-23.102012290906021</v>
       </c>
-      <c r="L24" s="3">
+      <c r="M24" s="3">
         <v>9000</v>
       </c>
-      <c r="M24">
-        <f>M13*100</f>
+      <c r="O24">
+        <f>O13*100</f>
         <v>212.39699999999999</v>
       </c>
-      <c r="N24">
-        <f t="shared" ref="N24:N27" si="12">M24/$L$1</f>
+      <c r="Q24">
+        <f>O24/$M$1</f>
         <v>2.6716603773584904</v>
       </c>
-      <c r="O24">
-        <f t="shared" ref="O24:O27" si="13">LN(N24)</f>
+      <c r="S24">
+        <f t="shared" ref="S24:S27" si="13">LN(Q24)</f>
         <v>0.98270014331396338</v>
       </c>
-      <c r="P24">
-        <f t="shared" ref="P24:P27" si="14">$L$1/L24</f>
+      <c r="T24">
+        <f>$M$1/M24</f>
         <v>8.8333333333333337E-3</v>
       </c>
-      <c r="Q24">
-        <f>P24*1000</f>
+      <c r="U24">
+        <f>T24*1000</f>
         <v>8.8333333333333339</v>
       </c>
-      <c r="T24" s="3">
+      <c r="X24" s="3">
         <v>9000</v>
       </c>
-      <c r="U24">
-        <f>U13*100</f>
+      <c r="Y24">
+        <f>Y13*100</f>
         <v>185.24799999999999</v>
       </c>
-      <c r="V24">
-        <f t="shared" ref="V24:V27" si="15">U24/$L$1</f>
+      <c r="Z24">
+        <f t="shared" ref="Z24:Z27" si="14">Y24/$M$1</f>
         <v>2.3301635220125787</v>
       </c>
-      <c r="W24">
-        <f t="shared" ref="W24:W27" si="16">LN(V24)</f>
+      <c r="AA24">
+        <f t="shared" ref="AA24:AA27" si="15">LN(Z24)</f>
         <v>0.84593844623630798</v>
       </c>
-      <c r="X24">
-        <f t="shared" ref="X24:X27" si="17">$L$1/T24</f>
+      <c r="AB24">
+        <f t="shared" ref="AB24:AB27" si="16">$M$1/X24</f>
         <v>8.8333333333333337E-3</v>
       </c>
-      <c r="Y24">
-        <f t="shared" ref="Y24:Y27" si="18">X24*1000</f>
+      <c r="AC24">
+        <f t="shared" ref="AC24:AC27" si="17">AB24*1000</f>
         <v>8.8333333333333339</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>103</v>
       </c>
       <c r="B25" s="1">
         <v>0.2</v>
       </c>
       <c r="C25">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
+      <c r="D25">
         <f t="shared" si="9"/>
-        <v>16</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>57.333333333333336</v>
       </c>
       <c r="F25">
@@ -2271,102 +2343,102 @@
         <f t="shared" si="4"/>
         <v>-23.582138927783205</v>
       </c>
-      <c r="L25" s="3">
+      <c r="M25" s="3">
         <v>10000</v>
       </c>
-      <c r="M25">
-        <f>M15*100</f>
+      <c r="O25">
+        <f>O15*100</f>
         <v>242.773</v>
       </c>
-      <c r="N25">
-        <f t="shared" si="12"/>
+      <c r="Q25">
+        <f>O25/$M$1</f>
         <v>3.0537484276729558</v>
       </c>
-      <c r="O25">
+      <c r="S25">
         <f t="shared" si="13"/>
         <v>1.1163698287056711</v>
       </c>
-      <c r="P25">
+      <c r="T25">
+        <f>$M$1/M25</f>
+        <v>7.9500000000000005E-3</v>
+      </c>
+      <c r="U25">
+        <f>T25*1000</f>
+        <v>7.95</v>
+      </c>
+      <c r="X25" s="3">
+        <v>10000</v>
+      </c>
+      <c r="Y25">
+        <f>Y15*100</f>
+        <v>206.71499999999997</v>
+      </c>
+      <c r="Z25">
         <f t="shared" si="14"/>
+        <v>2.6001886792452829</v>
+      </c>
+      <c r="AA25">
+        <f t="shared" si="15"/>
+        <v>0.95558401133493154</v>
+      </c>
+      <c r="AB25">
+        <f t="shared" si="16"/>
         <v>7.9500000000000005E-3</v>
       </c>
-      <c r="Q25">
-        <f>P25*1000</f>
+      <c r="AC25">
+        <f t="shared" si="17"/>
         <v>7.95</v>
       </c>
-      <c r="T25" s="3">
-        <v>10000</v>
-      </c>
-      <c r="U25">
-        <f>U15*100</f>
-        <v>206.71499999999997</v>
-      </c>
-      <c r="V25">
-        <f t="shared" si="15"/>
-        <v>2.6001886792452829</v>
-      </c>
-      <c r="W25">
-        <f t="shared" si="16"/>
-        <v>0.95558401133493154</v>
-      </c>
-      <c r="X25">
-        <f t="shared" si="17"/>
-        <v>7.9500000000000005E-3</v>
-      </c>
-      <c r="Y25">
-        <f t="shared" si="18"/>
-        <v>7.95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="L26" s="3">
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="M26" s="3">
         <v>11000</v>
       </c>
-      <c r="M26">
-        <f>M17*100</f>
+      <c r="O26">
+        <f>O17*100</f>
         <v>259.81700000000001</v>
       </c>
-      <c r="N26">
-        <f t="shared" si="12"/>
+      <c r="Q26">
+        <f>O26/$M$1</f>
         <v>3.2681383647798743</v>
       </c>
-      <c r="O26">
+      <c r="S26">
         <f t="shared" si="13"/>
         <v>1.1842205153854015</v>
       </c>
-      <c r="P26">
-        <f t="shared" si="14"/>
+      <c r="T26">
+        <f>$M$1/M26</f>
         <v>7.2272727272727271E-3</v>
       </c>
-      <c r="Q26">
-        <f>P26*1000</f>
+      <c r="U26">
+        <f>T26*1000</f>
         <v>7.2272727272727275</v>
       </c>
-      <c r="T26" s="3">
+      <c r="X26" s="3">
         <v>11000</v>
       </c>
-      <c r="U26">
-        <f>U17*100</f>
+      <c r="Y26">
+        <f>Y17*100</f>
         <v>228.404</v>
       </c>
-      <c r="V26">
-        <f>U26/$L$1</f>
+      <c r="Z26">
+        <f>Y26/$M$1</f>
         <v>2.8730062893081763</v>
       </c>
-      <c r="W26">
+      <c r="AA26">
+        <f t="shared" si="15"/>
+        <v>1.0553589691030669</v>
+      </c>
+      <c r="AB26">
         <f t="shared" si="16"/>
-        <v>1.0553589691030669</v>
-      </c>
-      <c r="X26">
+        <v>7.2272727272727271E-3</v>
+      </c>
+      <c r="AC26">
         <f t="shared" si="17"/>
-        <v>7.2272727272727271E-3</v>
-      </c>
-      <c r="Y26">
-        <f t="shared" si="18"/>
         <v>7.2272727272727275</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>0</v>
       </c>
@@ -2376,54 +2448,54 @@
       <c r="D27" t="s">
         <v>4</v>
       </c>
-      <c r="L27" s="3">
+      <c r="M27" s="3">
         <v>12000</v>
       </c>
-      <c r="M27">
-        <f>M19*100</f>
+      <c r="O27">
+        <f>O19*100</f>
         <v>291.37099999999998</v>
       </c>
-      <c r="N27">
-        <f t="shared" si="12"/>
+      <c r="Q27">
+        <f>O27/$M$1</f>
         <v>3.6650440251572323</v>
       </c>
-      <c r="O27">
+      <c r="S27">
         <f t="shared" si="13"/>
         <v>1.2988403475876769</v>
       </c>
-      <c r="P27">
+      <c r="T27">
+        <f>$M$1/M27</f>
+        <v>6.6249999999999998E-3</v>
+      </c>
+      <c r="U27">
+        <f>T27*1000</f>
+        <v>6.625</v>
+      </c>
+      <c r="X27" s="3">
+        <v>12000</v>
+      </c>
+      <c r="Y27">
+        <f>Y19*100</f>
+        <v>278.17500000000001</v>
+      </c>
+      <c r="Z27">
         <f t="shared" si="14"/>
+        <v>3.4990566037735849</v>
+      </c>
+      <c r="AA27">
+        <f t="shared" si="15"/>
+        <v>1.2524933903834781</v>
+      </c>
+      <c r="AB27">
+        <f t="shared" si="16"/>
         <v>6.6249999999999998E-3</v>
       </c>
-      <c r="Q27">
-        <f>P27*1000</f>
+      <c r="AC27">
+        <f t="shared" si="17"/>
         <v>6.625</v>
       </c>
-      <c r="T27" s="3">
-        <v>12000</v>
-      </c>
-      <c r="U27">
-        <f>U19*100</f>
-        <v>278.17500000000001</v>
-      </c>
-      <c r="V27">
-        <f t="shared" si="15"/>
-        <v>3.4990566037735849</v>
-      </c>
-      <c r="W27">
-        <f t="shared" si="16"/>
-        <v>1.2524933903834781</v>
-      </c>
-      <c r="X27">
-        <f t="shared" si="17"/>
-        <v>6.6249999999999998E-3</v>
-      </c>
-      <c r="Y27">
-        <f t="shared" si="18"/>
-        <v>6.625</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -2440,7 +2512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>85</f>
         <v>85</v>
@@ -2453,7 +2525,7 @@
         <v>180</v>
       </c>
       <c r="D29">
-        <f t="shared" ref="D29:D38" si="19">C29/2</f>
+        <f t="shared" ref="D29:D38" si="18">C29/2</f>
         <v>90</v>
       </c>
       <c r="E29" s="2">
@@ -2481,40 +2553,41 @@
         <f t="shared" si="4"/>
         <v>-20.112413899113296</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>34</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29"/>
+      <c r="O29" t="s">
         <v>35</v>
       </c>
-      <c r="N29">
+      <c r="Q29">
         <v>2.1948500000000002</v>
       </c>
-      <c r="P29" t="s">
+      <c r="T29" t="s">
         <v>19</v>
       </c>
-      <c r="Q29">
-        <f>EXP(N29)</f>
+      <c r="U29">
+        <f>EXP(Q29)</f>
         <v>8.9786541576808094</v>
       </c>
-      <c r="T29" t="s">
+      <c r="X29" t="s">
         <v>34</v>
       </c>
-      <c r="U29" t="s">
+      <c r="Y29" t="s">
         <v>35</v>
       </c>
-      <c r="V29">
+      <c r="Z29">
         <v>2.2303099999999998</v>
       </c>
-      <c r="X29" t="s">
+      <c r="AB29" t="s">
         <v>19</v>
       </c>
-      <c r="Y29">
-        <f>EXP(V29)</f>
+      <c r="AC29">
+        <f>EXP(Z29)</f>
         <v>9.302749484872967</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>A29+2</f>
         <v>87</v>
@@ -2523,15 +2596,15 @@
         <v>1.8</v>
       </c>
       <c r="C30">
-        <f t="shared" ref="C30:C38" si="20">C$27*$B30</f>
+        <f t="shared" ref="C30:C38" si="19">C$27*$B30</f>
         <v>162</v>
       </c>
       <c r="D30">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>81</v>
       </c>
       <c r="E30" s="2">
-        <f t="shared" ref="E30:E38" si="21">AVERAGE(F30,G30,H30)</f>
+        <f t="shared" ref="E30:E38" si="20">AVERAGE(F30,G30,H30)</f>
         <v>1247.6666666666667</v>
       </c>
       <c r="F30">
@@ -2548,73 +2621,75 @@
         <v>1.2476666666666668E-9</v>
       </c>
       <c r="J30" s="3">
-        <f t="shared" ref="J30:J64" si="22">LN(E30)</f>
+        <f t="shared" ref="J30:J64" si="21">LN(E30)</f>
         <v>7.1290304192363196</v>
       </c>
       <c r="K30" s="3">
         <f t="shared" si="4"/>
         <v>-20.501990696692229</v>
       </c>
-      <c r="L30"/>
-      <c r="M30" s="3" t="s">
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="N30">
+      <c r="P30" s="3"/>
+      <c r="Q30">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="P30" s="3" t="s">
+      <c r="T30" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Q30">
-        <f>EXP(N30)</f>
+      <c r="U30">
+        <f>EXP(Q30)</f>
         <v>1.0470744109569372</v>
       </c>
-      <c r="R30" t="s">
+      <c r="V30" t="s">
         <v>38</v>
       </c>
-      <c r="S30">
-        <f>Q30/Q29</f>
+      <c r="W30">
+        <f>U30/U29</f>
         <v>0.11661819160962059</v>
       </c>
-      <c r="U30" s="3" t="s">
+      <c r="Y30" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="V30">
+      <c r="Z30">
         <v>0.15090000000000001</v>
       </c>
-      <c r="X30" s="3" t="s">
+      <c r="AB30" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Y30">
-        <f>EXP(V30)</f>
+      <c r="AC30">
+        <f>EXP(Z30)</f>
         <v>1.1628803642308014</v>
       </c>
-      <c r="Z30" t="s">
+      <c r="AD30" t="s">
         <v>38</v>
       </c>
-      <c r="AA30">
-        <f>Y30/Y29</f>
+      <c r="AE30">
+        <f>AC30/AC29</f>
         <v>0.12500394277216001</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" ref="A31:A38" si="23">A30+2</f>
+        <f t="shared" ref="A31:A38" si="22">A30+2</f>
         <v>89</v>
       </c>
       <c r="B31" s="1">
         <v>1.6</v>
       </c>
       <c r="C31">
+        <f t="shared" si="19"/>
+        <v>144</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="18"/>
+        <v>72</v>
+      </c>
+      <c r="E31" s="2">
         <f t="shared" si="20"/>
-        <v>144</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="19"/>
-        <v>72</v>
-      </c>
-      <c r="E31" s="2">
-        <f t="shared" si="21"/>
         <v>898.66666666666663</v>
       </c>
       <c r="F31">
@@ -2631,59 +2706,60 @@
         <v>8.9866666666666667E-10</v>
       </c>
       <c r="J31" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>6.8009121833640878</v>
       </c>
       <c r="K31" s="3">
         <f t="shared" si="4"/>
         <v>-20.83010893256446</v>
       </c>
-      <c r="L31"/>
-      <c r="M31" t="s">
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31" t="s">
         <v>36</v>
       </c>
-      <c r="N31">
+      <c r="Q31">
         <v>-0.13697000000000001</v>
       </c>
-      <c r="P31" t="s">
+      <c r="T31" t="s">
         <v>20</v>
       </c>
-      <c r="Q31">
-        <f>N31*-1*1000</f>
+      <c r="U31">
+        <f>Q31*-1*1000</f>
         <v>136.97</v>
       </c>
-      <c r="U31" t="s">
+      <c r="Y31" t="s">
         <v>36</v>
       </c>
-      <c r="V31">
+      <c r="Z31">
         <v>-0.15629999999999999</v>
       </c>
-      <c r="X31" t="s">
+      <c r="AB31" t="s">
         <v>20</v>
       </c>
-      <c r="Y31">
-        <f>V31*-1*1000</f>
+      <c r="AC31">
+        <f>Z31*-1*1000</f>
         <v>156.29999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>91</v>
       </c>
       <c r="B32" s="1">
         <v>1.4</v>
       </c>
       <c r="C32">
+        <f t="shared" si="19"/>
+        <v>125.99999999999999</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="18"/>
+        <v>62.999999999999993</v>
+      </c>
+      <c r="E32" s="2">
         <f t="shared" si="20"/>
-        <v>125.99999999999999</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="19"/>
-        <v>62.999999999999993</v>
-      </c>
-      <c r="E32" s="2">
-        <f t="shared" si="21"/>
         <v>629.33333333333337</v>
       </c>
       <c r="F32">
@@ -2700,73 +2776,75 @@
         <v>6.2933333333333333E-10</v>
       </c>
       <c r="J32" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>6.4446610580373367</v>
       </c>
       <c r="K32" s="3">
         <f t="shared" si="4"/>
         <v>-21.186360057891211</v>
       </c>
-      <c r="L32"/>
-      <c r="M32" s="3" t="s">
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="N32">
+      <c r="P32" s="3"/>
+      <c r="Q32">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="P32" s="3" t="s">
+      <c r="T32" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Q32" s="6">
-        <f>N32*1000</f>
+      <c r="U32" s="6">
+        <f>Q32*1000</f>
         <v>5</v>
       </c>
-      <c r="R32" t="s">
+      <c r="V32" t="s">
         <v>38</v>
       </c>
-      <c r="S32">
-        <f>Q32/Q31</f>
+      <c r="W32">
+        <f>U32/U31</f>
         <v>3.6504344016938015E-2</v>
       </c>
-      <c r="U32" s="3" t="s">
+      <c r="Y32" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="V32">
+      <c r="Z32">
         <v>1.8409999999999999E-2</v>
       </c>
-      <c r="X32" s="3" t="s">
+      <c r="AB32" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Y32">
-        <f>V32*1000</f>
+      <c r="AC32">
+        <f>Z32*1000</f>
         <v>18.41</v>
       </c>
-      <c r="Z32" t="s">
+      <c r="AD32" t="s">
         <v>38</v>
       </c>
-      <c r="AA32">
-        <f>Y32/Y31</f>
+      <c r="AE32">
+        <f>AC32/AC31</f>
         <v>0.117786308381318</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>93</v>
       </c>
       <c r="B33" s="1">
         <v>1.2</v>
       </c>
       <c r="C33">
+        <f t="shared" si="19"/>
+        <v>108</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="18"/>
+        <v>54</v>
+      </c>
+      <c r="E33" s="2">
         <f t="shared" si="20"/>
-        <v>108</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="19"/>
-        <v>54</v>
-      </c>
-      <c r="E33" s="2">
-        <f t="shared" si="21"/>
         <v>437</v>
       </c>
       <c r="F33">
@@ -2783,46 +2861,46 @@
         <v>4.3699999999999999E-10</v>
       </c>
       <c r="J33" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>6.0799331950955899</v>
       </c>
       <c r="K33" s="3">
         <f t="shared" si="4"/>
         <v>-21.551087920832959</v>
       </c>
-      <c r="P33" s="1" t="s">
+      <c r="T33" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q33" s="1">
-        <f>Q31/Q29</f>
+      <c r="U33" s="1">
+        <f>U31/U29</f>
         <v>15.255070258255655</v>
       </c>
-      <c r="X33" s="1" t="s">
+      <c r="AB33" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y33" s="1">
-        <f>Y31/Y29</f>
+      <c r="AC33" s="1">
+        <f>AC31/AC29</f>
         <v>16.80148436267757</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>95</v>
       </c>
       <c r="B34" s="1">
         <v>1</v>
       </c>
       <c r="C34">
+        <f t="shared" si="19"/>
+        <v>90</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="18"/>
+        <v>45</v>
+      </c>
+      <c r="E34" s="2">
         <f t="shared" si="20"/>
-        <v>90</v>
-      </c>
-      <c r="D34">
-        <f t="shared" si="19"/>
-        <v>45</v>
-      </c>
-      <c r="E34" s="2">
-        <f t="shared" si="21"/>
         <v>278.66666666666669</v>
       </c>
       <c r="F34">
@@ -2839,60 +2917,60 @@
         <v>2.7866666666666669E-10</v>
       </c>
       <c r="J34" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>5.6300163244165917</v>
       </c>
       <c r="K34" s="3">
         <f t="shared" si="4"/>
         <v>-22.001004791511956</v>
       </c>
-      <c r="P34" s="3" t="s">
+      <c r="T34" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Q34">
-        <f>Q33*S34</f>
+      <c r="U34">
+        <f>U33*W34</f>
         <v>1.8641402328251779</v>
       </c>
-      <c r="R34" t="s">
+      <c r="V34" t="s">
         <v>38</v>
       </c>
-      <c r="S34">
-        <f>SQRT((S30^2)+(S32^2))</f>
+      <c r="W34">
+        <f>SQRT((W30^2)+(W32^2))</f>
         <v>0.12219807587030632</v>
       </c>
-      <c r="X34" s="3" t="s">
+      <c r="AB34" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Y34">
-        <f>Y33*AA34</f>
+      <c r="AC34">
+        <f>AC33*AE34</f>
         <v>2.8857301488306701</v>
       </c>
-      <c r="Z34" t="s">
+      <c r="AD34" t="s">
         <v>38</v>
       </c>
-      <c r="AA34">
-        <f>SQRT((AA30^2)+(AA32^2))</f>
+      <c r="AE34">
+        <f>SQRT((AE30^2)+(AE32^2))</f>
         <v>0.17175447636287211</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>97</v>
       </c>
       <c r="B35" s="1">
         <v>0.8</v>
       </c>
       <c r="C35">
+        <f t="shared" si="19"/>
+        <v>72</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="18"/>
+        <v>36</v>
+      </c>
+      <c r="E35" s="2">
         <f t="shared" si="20"/>
-        <v>72</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="19"/>
-        <v>36</v>
-      </c>
-      <c r="E35" s="2">
-        <f t="shared" si="21"/>
         <v>187.66666666666666</v>
       </c>
       <c r="F35">
@@ -2909,7 +2987,7 @@
         <v>1.8766666666666666E-10</v>
       </c>
       <c r="J35" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>5.2346673394715806</v>
       </c>
       <c r="K35" s="3">
@@ -2917,24 +2995,24 @@
         <v>-22.396353776456966</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>99</v>
       </c>
       <c r="B36" s="1">
         <v>0.6</v>
       </c>
       <c r="C36">
+        <f t="shared" si="19"/>
+        <v>54</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="18"/>
+        <v>27</v>
+      </c>
+      <c r="E36" s="2">
         <f t="shared" si="20"/>
-        <v>54</v>
-      </c>
-      <c r="D36">
-        <f t="shared" si="19"/>
-        <v>27</v>
-      </c>
-      <c r="E36" s="2">
-        <f t="shared" si="21"/>
         <v>121</v>
       </c>
       <c r="F36">
@@ -2951,46 +3029,46 @@
         <v>1.21E-10</v>
       </c>
       <c r="J36" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>4.7957905455967413</v>
       </c>
       <c r="K36" s="3">
         <f t="shared" si="4"/>
         <v>-22.835230570331806</v>
       </c>
-      <c r="N36" t="s">
+      <c r="Q36" t="s">
         <v>39</v>
       </c>
-      <c r="O36">
+      <c r="S36">
         <v>15.76</v>
       </c>
-      <c r="Q36">
-        <f>O36-Q33</f>
+      <c r="U36">
+        <f>S36-U33</f>
         <v>0.5049297417443448</v>
       </c>
-      <c r="Y36">
-        <f>Y33-O36</f>
+      <c r="AC36">
+        <f>AC33-S36</f>
         <v>1.0414843626775703</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>101</v>
       </c>
       <c r="B37" s="1">
         <v>0.4</v>
       </c>
       <c r="C37">
+        <f t="shared" si="19"/>
+        <v>36</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="18"/>
+        <v>18</v>
+      </c>
+      <c r="E37" s="2">
         <f t="shared" si="20"/>
-        <v>36</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="19"/>
-        <v>18</v>
-      </c>
-      <c r="E37" s="2">
-        <f t="shared" si="21"/>
         <v>72</v>
       </c>
       <c r="F37">
@@ -3007,35 +3085,35 @@
         <v>7.1999999999999997E-11</v>
       </c>
       <c r="J37" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>4.2766661190160553</v>
       </c>
       <c r="K37" s="3">
         <f t="shared" si="4"/>
         <v>-23.354354996912495</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="U37" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>103</v>
       </c>
       <c r="B38" s="1">
         <v>0.2</v>
       </c>
       <c r="C38">
+        <f t="shared" si="19"/>
+        <v>18</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="18"/>
+        <v>9</v>
+      </c>
+      <c r="E38" s="2">
         <f t="shared" si="20"/>
-        <v>18</v>
-      </c>
-      <c r="D38">
-        <f t="shared" si="19"/>
-        <v>9</v>
-      </c>
-      <c r="E38" s="2">
-        <f t="shared" si="21"/>
         <v>33.666666666666664</v>
       </c>
       <c r="F38">
@@ -3052,7 +3130,7 @@
         <v>3.3666666666666667E-11</v>
       </c>
       <c r="J38" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>3.5165082281731497</v>
       </c>
       <c r="K38" s="3">
@@ -3060,7 +3138,7 @@
         <v>-24.114512887755399</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>0</v>
       </c>
@@ -3071,7 +3149,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -3088,7 +3166,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42">
         <f>85</f>
         <v>85</v>
@@ -3101,7 +3179,7 @@
         <v>220</v>
       </c>
       <c r="D42">
-        <f t="shared" ref="D42:D51" si="24">C42/2</f>
+        <f t="shared" ref="D42:D51" si="23">C42/2</f>
         <v>110</v>
       </c>
       <c r="E42" s="2">
@@ -3122,7 +3200,7 @@
         <v>1.9016666666666668E-9</v>
       </c>
       <c r="J42" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>7.5504859736280663</v>
       </c>
       <c r="K42" s="3">
@@ -3130,7 +3208,7 @@
         <v>-20.08053514230048</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43">
         <f>A42+2</f>
         <v>87</v>
@@ -3139,15 +3217,15 @@
         <v>1.8</v>
       </c>
       <c r="C43">
-        <f t="shared" ref="C43:C51" si="25">C$40*$B43</f>
+        <f t="shared" ref="C43:C51" si="24">C$40*$B43</f>
         <v>198</v>
       </c>
       <c r="D43">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>99</v>
       </c>
       <c r="E43" s="2">
-        <f t="shared" ref="E43:E51" si="26">AVERAGE(F43,G43,H43)</f>
+        <f t="shared" ref="E43:E51" si="25">AVERAGE(F43,G43,H43)</f>
         <v>1243.6666666666667</v>
       </c>
       <c r="F43">
@@ -3164,40 +3242,38 @@
         <v>1.2436666666666668E-9</v>
       </c>
       <c r="J43" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>7.1258192845530486</v>
       </c>
       <c r="K43" s="3">
         <f t="shared" si="4"/>
         <v>-20.505201831375501</v>
       </c>
-      <c r="M43" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="N43" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="O43" s="14"/>
-      <c r="P43" s="16"/>
-    </row>
-    <row r="44" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O43" s="7"/>
+      <c r="P43" s="24"/>
+      <c r="Q43" s="17"/>
+      <c r="R43" s="18"/>
+      <c r="S43" s="18"/>
+      <c r="T43" s="19"/>
+    </row>
+    <row r="44" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" ref="A44:A51" si="27">A43+2</f>
+        <f t="shared" ref="A44:A51" si="26">A43+2</f>
         <v>89</v>
       </c>
       <c r="B44" s="1">
         <v>1.6</v>
       </c>
       <c r="C44">
+        <f t="shared" si="24"/>
+        <v>176</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="23"/>
+        <v>88</v>
+      </c>
+      <c r="E44" s="2">
         <f t="shared" si="25"/>
-        <v>176</v>
-      </c>
-      <c r="D44">
-        <f t="shared" si="24"/>
-        <v>88</v>
-      </c>
-      <c r="E44" s="2">
-        <f t="shared" si="26"/>
         <v>785.66666666666663</v>
       </c>
       <c r="F44">
@@ -3214,40 +3290,38 @@
         <v>7.8566666666666664E-10</v>
       </c>
       <c r="J44" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>6.6665326142680215</v>
       </c>
       <c r="K44" s="3">
         <f t="shared" si="4"/>
         <v>-20.964488501660526</v>
       </c>
-      <c r="M44" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="N44" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="O44" s="18"/>
-      <c r="P44" s="19"/>
-    </row>
-    <row r="45" spans="1:27" ht="24" x14ac:dyDescent="0.25">
+      <c r="O44" s="8"/>
+      <c r="P44" s="25"/>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="21"/>
+      <c r="S44" s="21"/>
+      <c r="T44" s="22"/>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>91</v>
       </c>
       <c r="B45" s="1">
         <v>1.4</v>
       </c>
       <c r="C45">
+        <f t="shared" si="24"/>
+        <v>154</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="23"/>
+        <v>77</v>
+      </c>
+      <c r="E45" s="2">
         <f t="shared" si="25"/>
-        <v>154</v>
-      </c>
-      <c r="D45">
-        <f t="shared" si="24"/>
-        <v>77</v>
-      </c>
-      <c r="E45" s="2">
-        <f t="shared" si="26"/>
         <v>478</v>
       </c>
       <c r="F45">
@@ -3264,62 +3338,38 @@
         <v>4.78E-10</v>
       </c>
       <c r="J45" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>6.1696107324914564</v>
       </c>
       <c r="K45" s="3">
         <f t="shared" si="4"/>
         <v>-21.461410383437091</v>
       </c>
-      <c r="M45" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="N45" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="O45" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="P45" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="R45">
-        <v>80</v>
-      </c>
-      <c r="S45">
-        <v>100</v>
-      </c>
-      <c r="T45">
-        <v>120</v>
-      </c>
-      <c r="V45">
-        <v>80</v>
-      </c>
-      <c r="W45">
-        <v>100</v>
-      </c>
-      <c r="X45">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="46" spans="1:27" ht="24" x14ac:dyDescent="0.25">
+      <c r="O45" s="8"/>
+      <c r="P45" s="26"/>
+      <c r="Q45" s="9"/>
+      <c r="R45" s="9"/>
+      <c r="S45" s="9"/>
+      <c r="T45" s="10"/>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>93</v>
       </c>
       <c r="B46" s="1">
         <v>1.2</v>
       </c>
       <c r="C46">
+        <f t="shared" si="24"/>
+        <v>132</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="23"/>
+        <v>66</v>
+      </c>
+      <c r="E46" s="2">
         <f t="shared" si="25"/>
-        <v>132</v>
-      </c>
-      <c r="D46">
-        <f t="shared" si="24"/>
-        <v>66</v>
-      </c>
-      <c r="E46" s="2">
-        <f t="shared" si="26"/>
         <v>302</v>
       </c>
       <c r="F46">
@@ -3336,68 +3386,39 @@
         <v>3.0199999999999999E-10</v>
       </c>
       <c r="J46" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>5.7104270173748697</v>
       </c>
       <c r="K46" s="3">
         <f t="shared" si="4"/>
         <v>-21.920594098553678</v>
       </c>
-      <c r="M46" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="N46" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="O46" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="P46" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q46" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="R46">
-        <v>-14.43886</v>
-      </c>
-      <c r="S46">
-        <v>-16.115269999999999</v>
-      </c>
-      <c r="T46">
-        <v>-17.712630000000001</v>
-      </c>
-      <c r="V46">
-        <f>EXP(R46)</f>
-        <v>5.3614563805160336E-7</v>
-      </c>
-      <c r="W46">
-        <f t="shared" ref="W46:X47" si="28">EXP(S46)</f>
-        <v>1.0028296468727901E-7</v>
-      </c>
-      <c r="X46">
-        <f t="shared" si="28"/>
-        <v>2.0300303505511811E-8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:27" ht="24" x14ac:dyDescent="0.25">
+      <c r="O46" s="8"/>
+      <c r="P46" s="26"/>
+      <c r="Q46" s="9"/>
+      <c r="R46" s="9"/>
+      <c r="S46" s="9"/>
+      <c r="T46" s="10"/>
+      <c r="U46" s="16"/>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>95</v>
       </c>
       <c r="B47" s="1">
         <v>1</v>
       </c>
       <c r="C47">
+        <f t="shared" si="24"/>
+        <v>110</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="23"/>
+        <v>55</v>
+      </c>
+      <c r="E47" s="2">
         <f t="shared" si="25"/>
-        <v>110</v>
-      </c>
-      <c r="D47">
-        <f t="shared" si="24"/>
-        <v>55</v>
-      </c>
-      <c r="E47" s="2">
-        <f t="shared" si="26"/>
         <v>181</v>
       </c>
       <c r="F47">
@@ -3414,68 +3435,39 @@
         <v>1.81E-10</v>
       </c>
       <c r="J47" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>5.1984970312658261</v>
       </c>
       <c r="K47" s="3">
         <f t="shared" si="4"/>
         <v>-22.432524084662724</v>
       </c>
-      <c r="M47" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="N47" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="O47" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="P47" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q47" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="R47">
-        <v>-9.6077100000000009</v>
-      </c>
-      <c r="S47">
-        <v>-9.2610200000000003</v>
-      </c>
-      <c r="T47">
-        <v>-9.6968700000000005</v>
-      </c>
-      <c r="V47">
-        <f>EXP(R47)</f>
-        <v>6.7208555805853515E-5</v>
-      </c>
-      <c r="W47">
-        <f t="shared" si="28"/>
-        <v>9.5058316196068538E-5</v>
-      </c>
-      <c r="X47">
-        <f t="shared" si="28"/>
-        <v>6.1475612900322769E-5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:27" ht="24" x14ac:dyDescent="0.25">
+      <c r="O47" s="8"/>
+      <c r="P47" s="26"/>
+      <c r="Q47" s="9"/>
+      <c r="R47" s="9"/>
+      <c r="S47" s="9"/>
+      <c r="T47" s="10"/>
+      <c r="U47" s="16"/>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>97</v>
       </c>
       <c r="B48" s="1">
         <v>0.8</v>
       </c>
       <c r="C48">
+        <f t="shared" si="24"/>
+        <v>88</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="23"/>
+        <v>44</v>
+      </c>
+      <c r="E48" s="2">
         <f t="shared" si="25"/>
-        <v>88</v>
-      </c>
-      <c r="D48">
-        <f t="shared" si="24"/>
-        <v>44</v>
-      </c>
-      <c r="E48" s="2">
-        <f t="shared" si="26"/>
         <v>116</v>
       </c>
       <c r="F48">
@@ -3492,71 +3484,39 @@
         <v>1.16E-10</v>
       </c>
       <c r="J48" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>4.7535901911063645</v>
       </c>
       <c r="K48" s="3">
         <f t="shared" si="4"/>
         <v>-22.877430924822182</v>
       </c>
-      <c r="M48" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="N48" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="O48" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="P48" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q48" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="R48">
-        <v>-4.0106799999999998</v>
-      </c>
-      <c r="S48">
-        <v>-2.4928900000000001</v>
-      </c>
-      <c r="T48">
-        <v>-1.5214099999999999</v>
-      </c>
-      <c r="U48" t="s">
-        <v>77</v>
-      </c>
-      <c r="V48">
-        <f>EXP(1/R48)</f>
-        <v>0.77931942090725548</v>
-      </c>
-      <c r="W48">
-        <f t="shared" ref="W48:X48" si="29">EXP(1/S48)</f>
-        <v>0.66955575111011467</v>
-      </c>
-      <c r="X48">
-        <f t="shared" si="29"/>
-        <v>0.51825648291462234</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" ht="24" x14ac:dyDescent="0.25">
+      <c r="O48" s="8"/>
+      <c r="P48" s="26"/>
+      <c r="Q48" s="9"/>
+      <c r="R48" s="9"/>
+      <c r="S48" s="9"/>
+      <c r="T48" s="10"/>
+      <c r="U48" s="16"/>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>99</v>
       </c>
       <c r="B49" s="1">
         <v>0.6</v>
       </c>
       <c r="C49">
+        <f t="shared" si="24"/>
+        <v>66</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="23"/>
+        <v>33</v>
+      </c>
+      <c r="E49" s="2">
         <f t="shared" si="25"/>
-        <v>66</v>
-      </c>
-      <c r="D49">
-        <f t="shared" si="24"/>
-        <v>33</v>
-      </c>
-      <c r="E49" s="2">
-        <f t="shared" si="26"/>
         <v>66.666666666666671</v>
       </c>
       <c r="F49">
@@ -3573,44 +3533,38 @@
         <v>6.6666666666666669E-11</v>
       </c>
       <c r="J49" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>4.1997050778799272</v>
       </c>
       <c r="K49" s="3">
         <f t="shared" si="4"/>
         <v>-23.431316038048621</v>
       </c>
-      <c r="M49" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="N49" s="9">
-        <v>2.1800000000000001E-3</v>
-      </c>
-      <c r="O49" s="21">
-        <v>8.2982100000000001E-4</v>
-      </c>
-      <c r="P49" s="10">
-        <v>3.3579999999999999E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24" ht="24" x14ac:dyDescent="0.25">
+      <c r="O49" s="8"/>
+      <c r="P49" s="26"/>
+      <c r="Q49" s="9"/>
+      <c r="R49" s="9"/>
+      <c r="S49" s="15"/>
+      <c r="T49" s="10"/>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>101</v>
       </c>
       <c r="B50" s="1">
         <v>0.4</v>
       </c>
       <c r="C50">
+        <f t="shared" si="24"/>
+        <v>44</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="23"/>
+        <v>22</v>
+      </c>
+      <c r="E50" s="2">
         <f t="shared" si="25"/>
-        <v>44</v>
-      </c>
-      <c r="D50">
-        <f t="shared" si="24"/>
-        <v>22</v>
-      </c>
-      <c r="E50" s="2">
-        <f t="shared" si="26"/>
         <v>35.666666666666664</v>
       </c>
       <c r="F50">
@@ -3627,44 +3581,38 @@
         <v>3.5666666666666666E-11</v>
       </c>
       <c r="J50" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>3.5742165457937962</v>
       </c>
       <c r="K50" s="3">
         <f t="shared" si="4"/>
         <v>-24.056804570134751</v>
       </c>
-      <c r="M50" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="N50" s="9">
-        <v>0.99922</v>
-      </c>
-      <c r="O50" s="9">
-        <v>0.99948000000000004</v>
-      </c>
-      <c r="P50" s="10">
-        <v>0.99338000000000004</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="O50" s="8"/>
+      <c r="P50" s="26"/>
+      <c r="Q50" s="9"/>
+      <c r="R50" s="9"/>
+      <c r="S50" s="9"/>
+      <c r="T50" s="10"/>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>103</v>
       </c>
       <c r="B51" s="1">
         <v>0.2</v>
       </c>
       <c r="C51">
+        <f t="shared" si="24"/>
+        <v>22</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="23"/>
+        <v>11</v>
+      </c>
+      <c r="E51" s="2">
         <f t="shared" si="25"/>
-        <v>22</v>
-      </c>
-      <c r="D51">
-        <f t="shared" si="24"/>
-        <v>11</v>
-      </c>
-      <c r="E51" s="2">
-        <f t="shared" si="26"/>
         <v>14.666666666666666</v>
       </c>
       <c r="F51">
@@ -3681,42 +3629,25 @@
         <v>1.4666666666666664E-11</v>
       </c>
       <c r="J51" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>2.6855773452501515</v>
       </c>
       <c r="K51" s="3">
         <f t="shared" si="4"/>
         <v>-24.945443770678398</v>
       </c>
-      <c r="M51" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N51" s="12">
-        <v>0.999</v>
-      </c>
-      <c r="O51" s="12">
-        <v>0.99933000000000005</v>
-      </c>
-      <c r="P51" s="13">
-        <v>0.99148999999999998</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="M52" s="3"/>
-      <c r="T52">
-        <v>90</v>
-      </c>
-      <c r="U52">
-        <v>110</v>
-      </c>
-      <c r="W52">
-        <v>90</v>
-      </c>
-      <c r="X52">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="O51" s="11"/>
+      <c r="P51" s="27"/>
+      <c r="Q51" s="12"/>
+      <c r="R51" s="12"/>
+      <c r="S51" s="12"/>
+      <c r="T51" s="13"/>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="O52" s="3"/>
+      <c r="P52" s="3"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>0</v>
       </c>
@@ -3726,38 +3657,16 @@
       <c r="D53" t="s">
         <v>4</v>
       </c>
-      <c r="M53" s="3"/>
-      <c r="N53" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="O53" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="P53" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q53" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="S53" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="T53">
-        <v>-16.756959999999999</v>
-      </c>
-      <c r="U53">
-        <v>-14.63026</v>
-      </c>
-      <c r="W53">
-        <f>EXP(T53)</f>
-        <v>5.278915843438181E-8</v>
-      </c>
-      <c r="X53">
-        <f>EXP(U53)</f>
-        <v>4.4275024806557514E-7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24" ht="36" x14ac:dyDescent="0.25">
+      <c r="O53" s="3"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="7"/>
+      <c r="R53" s="24"/>
+      <c r="S53" s="14"/>
+      <c r="T53" s="7"/>
+      <c r="U53" s="14"/>
+      <c r="W53" s="16"/>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -3773,37 +3682,14 @@
       <c r="E54" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N54" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="O54" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="P54" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q54" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="S54" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="T54">
-        <v>-7.9023300000000001</v>
-      </c>
-      <c r="U54">
-        <v>-10.922510000000001</v>
-      </c>
-      <c r="W54">
-        <f>EXP(T54)</f>
-        <v>3.6988071359346714E-4</v>
-      </c>
-      <c r="X54">
-        <f>EXP(U54)</f>
-        <v>1.804738065106965E-5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:24" ht="24" x14ac:dyDescent="0.25">
+      <c r="Q54" s="8"/>
+      <c r="R54" s="25"/>
+      <c r="S54" s="10"/>
+      <c r="T54" s="8"/>
+      <c r="U54" s="10"/>
+      <c r="W54" s="16"/>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55">
         <f>85</f>
         <v>85</v>
@@ -3816,11 +3702,11 @@
         <v>240</v>
       </c>
       <c r="D55">
-        <f t="shared" ref="D55:D64" si="30">C55/2</f>
+        <f t="shared" ref="D55:D64" si="27">C55/2</f>
         <v>120</v>
       </c>
       <c r="E55" s="2">
-        <f t="shared" ref="E55:E64" si="31">AVERAGE(F55,G55,H55)</f>
+        <f t="shared" ref="E55:E64" si="28">AVERAGE(F55,G55,H55)</f>
         <v>1862.3333333333333</v>
       </c>
       <c r="F55">
@@ -3837,47 +3723,21 @@
         <v>1.8623333333333332E-9</v>
       </c>
       <c r="J55" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>7.5295854607910391</v>
       </c>
       <c r="K55" s="3">
         <f t="shared" si="4"/>
         <v>-20.101435655137511</v>
       </c>
-      <c r="N55" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="O55" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="P55" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q55" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="S55" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="T55">
-        <v>-2.3885200000000002</v>
-      </c>
-      <c r="U55">
-        <v>-2.9170400000000001</v>
-      </c>
-      <c r="V55" t="s">
-        <v>77</v>
-      </c>
-      <c r="W55">
-        <f>EXP(1/T55)</f>
-        <v>0.65792173303153134</v>
-      </c>
-      <c r="X55">
-        <f>EXP(1/U55)</f>
-        <v>0.70977073981517713</v>
-      </c>
-    </row>
-    <row r="56" spans="1:24" ht="24" x14ac:dyDescent="0.25">
+      <c r="Q55" s="8"/>
+      <c r="R55" s="25"/>
+      <c r="S55" s="10"/>
+      <c r="T55" s="8"/>
+      <c r="U55" s="10"/>
+      <c r="W55" s="16"/>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56">
         <f>A55+2</f>
         <v>87</v>
@@ -3886,15 +3746,15 @@
         <v>1.8</v>
       </c>
       <c r="C56">
-        <f t="shared" ref="C56:C64" si="32">C$53*$B56</f>
+        <f t="shared" ref="C56:C64" si="29">C$53*$B56</f>
         <v>216</v>
       </c>
       <c r="D56">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>108</v>
       </c>
       <c r="E56" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="28"/>
         <v>1043.6666666666667</v>
       </c>
       <c r="F56">
@@ -3911,44 +3771,37 @@
         <v>1.0436666666666667E-9</v>
       </c>
       <c r="J56" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>6.9504954326582959</v>
       </c>
       <c r="K56" s="3">
         <f t="shared" si="4"/>
         <v>-20.68052568327025</v>
       </c>
-      <c r="N56" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="O56" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="P56" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q56" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24" ht="24" x14ac:dyDescent="0.25">
+      <c r="Q56" s="8"/>
+      <c r="R56" s="25"/>
+      <c r="S56" s="10"/>
+      <c r="T56" s="8"/>
+      <c r="U56" s="10"/>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" ref="A57:A64" si="33">A56+2</f>
+        <f t="shared" ref="A57:A64" si="30">A56+2</f>
         <v>89</v>
       </c>
       <c r="B57" s="1">
         <v>1.6</v>
       </c>
       <c r="C57">
-        <f t="shared" si="32"/>
+        <f t="shared" si="29"/>
         <v>192</v>
       </c>
       <c r="D57">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>96</v>
       </c>
       <c r="E57" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="28"/>
         <v>598.66666666666663</v>
       </c>
       <c r="F57">
@@ -3965,44 +3818,37 @@
         <v>5.9866666666666667E-10</v>
       </c>
       <c r="J57" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>6.3947049601940353</v>
       </c>
       <c r="K57" s="3">
         <f t="shared" si="4"/>
         <v>-21.236316155734514</v>
       </c>
-      <c r="N57" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="O57" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="P57" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q57" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="58" spans="1:24" ht="24" x14ac:dyDescent="0.25">
+      <c r="Q57" s="8"/>
+      <c r="R57" s="25"/>
+      <c r="S57" s="10"/>
+      <c r="T57" s="8"/>
+      <c r="U57" s="10"/>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f t="shared" si="33"/>
+        <f t="shared" si="30"/>
         <v>91</v>
       </c>
       <c r="B58" s="1">
         <v>1.4</v>
       </c>
       <c r="C58">
-        <f t="shared" si="32"/>
+        <f t="shared" si="29"/>
         <v>168</v>
       </c>
       <c r="D58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>84</v>
       </c>
       <c r="E58" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="28"/>
         <v>353.66666666666669</v>
       </c>
       <c r="F58">
@@ -4019,44 +3865,37 @@
         <v>3.5366666666666669E-10</v>
       </c>
       <c r="J58" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>5.8683548499458738</v>
       </c>
       <c r="K58" s="3">
         <f t="shared" si="4"/>
         <v>-21.762666265982674</v>
       </c>
-      <c r="N58" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="O58" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="P58" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q58" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="59" spans="1:24" ht="24" x14ac:dyDescent="0.25">
+      <c r="Q58" s="8"/>
+      <c r="R58" s="25"/>
+      <c r="S58" s="10"/>
+      <c r="T58" s="8"/>
+      <c r="U58" s="10"/>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="33"/>
+        <f t="shared" si="30"/>
         <v>93</v>
       </c>
       <c r="B59" s="1">
         <v>1.2</v>
       </c>
       <c r="C59">
-        <f t="shared" si="32"/>
+        <f t="shared" si="29"/>
         <v>144</v>
       </c>
       <c r="D59">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>72</v>
       </c>
       <c r="E59" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="28"/>
         <v>224.66666666666666</v>
       </c>
       <c r="F59">
@@ -4073,44 +3912,37 @@
         <v>2.2466666666666667E-10</v>
       </c>
       <c r="J59" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>5.414617822244197</v>
       </c>
       <c r="K59" s="3">
         <f t="shared" si="4"/>
         <v>-22.216403293684351</v>
       </c>
-      <c r="N59" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="O59" s="10">
-        <v>4.1999999999999997E-3</v>
-      </c>
-      <c r="P59" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q59" s="10">
-        <v>6.8700000000000002E-3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:24" ht="24" x14ac:dyDescent="0.25">
+      <c r="Q59" s="8"/>
+      <c r="R59" s="25"/>
+      <c r="S59" s="10"/>
+      <c r="T59" s="8"/>
+      <c r="U59" s="10"/>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="33"/>
+        <f t="shared" si="30"/>
         <v>95</v>
       </c>
       <c r="B60" s="1">
         <v>1</v>
       </c>
       <c r="C60">
-        <f t="shared" si="32"/>
+        <f t="shared" si="29"/>
         <v>120</v>
       </c>
       <c r="D60">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>60</v>
       </c>
       <c r="E60" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="28"/>
         <v>125</v>
       </c>
       <c r="F60">
@@ -4127,44 +3959,37 @@
         <v>1.2500000000000001E-10</v>
       </c>
       <c r="J60" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>4.8283137373023015</v>
       </c>
       <c r="K60" s="3">
         <f t="shared" si="4"/>
         <v>-22.802707378626248</v>
       </c>
-      <c r="N60" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="O60" s="10">
-        <v>0.99804999999999999</v>
-      </c>
-      <c r="P60" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q60" s="10">
-        <v>0.99785999999999997</v>
-      </c>
-    </row>
-    <row r="61" spans="1:24" ht="24" x14ac:dyDescent="0.25">
+      <c r="Q60" s="8"/>
+      <c r="R60" s="25"/>
+      <c r="S60" s="10"/>
+      <c r="T60" s="8"/>
+      <c r="U60" s="10"/>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f t="shared" si="33"/>
+        <f t="shared" si="30"/>
         <v>97</v>
       </c>
       <c r="B61" s="1">
         <v>0.8</v>
       </c>
       <c r="C61">
-        <f t="shared" si="32"/>
+        <f t="shared" si="29"/>
         <v>96</v>
       </c>
       <c r="D61">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>48</v>
       </c>
       <c r="E61" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="28"/>
         <v>76.333333333333329</v>
       </c>
       <c r="F61">
@@ -4181,44 +4006,37 @@
         <v>7.6333333333333328E-11</v>
       </c>
       <c r="J61" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>4.33510971488613</v>
       </c>
       <c r="K61" s="3">
         <f t="shared" si="4"/>
         <v>-23.295911401042417</v>
       </c>
-      <c r="N61" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="O61" s="13">
-        <v>0.99748999999999999</v>
-      </c>
-      <c r="P61" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q61" s="13">
-        <v>0.99724999999999997</v>
-      </c>
-    </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Q61" s="11"/>
+      <c r="R61" s="28"/>
+      <c r="S61" s="13"/>
+      <c r="T61" s="11"/>
+      <c r="U61" s="13"/>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62">
-        <f t="shared" si="33"/>
+        <f t="shared" si="30"/>
         <v>99</v>
       </c>
       <c r="B62" s="1">
         <v>0.6</v>
       </c>
       <c r="C62">
-        <f t="shared" si="32"/>
+        <f t="shared" si="29"/>
         <v>72</v>
       </c>
       <c r="D62">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>36</v>
       </c>
       <c r="E62" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="28"/>
         <v>34.333333333333336</v>
       </c>
       <c r="F62">
@@ -4235,7 +4053,7 @@
         <v>3.4333333333333338E-11</v>
       </c>
       <c r="J62" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>3.5361166995615263</v>
       </c>
       <c r="K62" s="3">
@@ -4243,24 +4061,24 @@
         <v>-24.094904416367022</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63">
-        <f t="shared" si="33"/>
+        <f t="shared" si="30"/>
         <v>101</v>
       </c>
       <c r="B63" s="1">
         <v>0.4</v>
       </c>
       <c r="C63">
-        <f t="shared" si="32"/>
+        <f t="shared" si="29"/>
         <v>48</v>
       </c>
       <c r="D63">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>24</v>
       </c>
       <c r="E63" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="28"/>
         <v>14</v>
       </c>
       <c r="F63">
@@ -4277,7 +4095,7 @@
         <v>1.4E-11</v>
       </c>
       <c r="J63" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>2.6390573296152584</v>
       </c>
       <c r="K63" s="3">
@@ -4285,24 +4103,24 @@
         <v>-24.991963786313288</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="30"/>
         <v>103</v>
       </c>
       <c r="B64" s="1">
         <v>0.2</v>
       </c>
       <c r="C64">
-        <f t="shared" si="32"/>
+        <f t="shared" si="29"/>
         <v>24</v>
       </c>
       <c r="D64">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>12</v>
       </c>
       <c r="E64" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="28"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="F64">
@@ -4319,7 +4137,7 @@
         <v>3.3333333333333335E-12</v>
       </c>
       <c r="J64" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>1.2039728043259361</v>
       </c>
       <c r="K64" s="3">
@@ -4327,10 +4145,721 @@
         <v>-26.427048311602611</v>
       </c>
     </row>
+    <row r="69" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="70" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B70" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D70" s="18"/>
+      <c r="E70" s="19"/>
+      <c r="G70" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H70" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="I70" s="19"/>
+    </row>
+    <row r="71" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B71" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C71" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D71" s="21"/>
+      <c r="E71" s="22"/>
+      <c r="G71" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H71" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I71" s="22"/>
+    </row>
+    <row r="72" spans="2:20" ht="24" x14ac:dyDescent="0.25">
+      <c r="B72" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G72" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H72" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I72" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="K72" s="29">
+        <v>80</v>
+      </c>
+      <c r="L72" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="M72" s="29">
+        <v>90</v>
+      </c>
+      <c r="N72" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="O72" s="29">
+        <v>100</v>
+      </c>
+      <c r="P72" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q72" s="30">
+        <v>110</v>
+      </c>
+      <c r="R72" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="S72" s="30">
+        <v>120</v>
+      </c>
+      <c r="T72" s="29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="73" spans="2:20" ht="24" x14ac:dyDescent="0.25">
+      <c r="B73" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I73" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J73" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K73" s="6">
+        <v>1.60012</v>
+      </c>
+      <c r="L73" s="6">
+        <v>5.4940000000000003E-2</v>
+      </c>
+      <c r="M73" s="6">
+        <v>1.69129</v>
+      </c>
+      <c r="N73" s="6">
+        <v>2.7300000000000001E-2</v>
+      </c>
+      <c r="O73" s="6">
+        <v>2.03335</v>
+      </c>
+      <c r="P73" s="6">
+        <v>3.6569999999999998E-2</v>
+      </c>
+      <c r="Q73" s="6">
+        <v>2.21671</v>
+      </c>
+      <c r="R73" s="6">
+        <v>2.5839999999999998E-2</v>
+      </c>
+      <c r="S73" s="6">
+        <v>2.57037</v>
+      </c>
+      <c r="T73" s="6">
+        <v>5.3460000000000001E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="2:20" ht="48" x14ac:dyDescent="0.25">
+      <c r="B74" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G74" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H74" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I74" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="J74" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K74" s="29">
+        <v>6.7391899999999998E-11</v>
+      </c>
+      <c r="L74" s="29">
+        <v>6.3372999999999997E-12</v>
+      </c>
+      <c r="M74" s="29">
+        <v>6.3460899999999996E-11</v>
+      </c>
+      <c r="N74" s="29">
+        <v>2.8329099999999999E-12</v>
+      </c>
+      <c r="O74" s="29">
+        <v>2.9477299999999997E-11</v>
+      </c>
+      <c r="P74" s="29">
+        <v>1.67729E-12</v>
+      </c>
+      <c r="Q74" s="29">
+        <v>2.28835E-11</v>
+      </c>
+      <c r="R74" s="29">
+        <v>9.0111900000000003E-13</v>
+      </c>
+      <c r="S74" s="29">
+        <v>1.0552500000000001E-11</v>
+      </c>
+      <c r="T74" s="29">
+        <v>8.0733500000000001E-13</v>
+      </c>
+    </row>
+    <row r="75" spans="2:20" ht="48" x14ac:dyDescent="0.25">
+      <c r="B75" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G75" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H75" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I75" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="J75" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K75" s="29">
+        <v>-3.6142799999999998E-11</v>
+      </c>
+      <c r="L75" s="29">
+        <v>8.9411000000000003E-12</v>
+      </c>
+      <c r="M75" s="29">
+        <v>-5.4948099999999997E-11</v>
+      </c>
+      <c r="N75" s="29">
+        <v>3.8618999999999999E-12</v>
+      </c>
+      <c r="O75" s="29">
+        <v>-2.6070299999999999E-11</v>
+      </c>
+      <c r="P75" s="29">
+        <v>2.4865899999999998E-12</v>
+      </c>
+      <c r="Q75" s="29">
+        <v>-2.0799799999999999E-11</v>
+      </c>
+      <c r="R75" s="29">
+        <v>1.3931400000000001E-12</v>
+      </c>
+      <c r="S75" s="29">
+        <v>-1.4355199999999999E-11</v>
+      </c>
+      <c r="T75" s="29">
+        <v>1.2215099999999999E-12</v>
+      </c>
+    </row>
+    <row r="76" spans="2:20" ht="24" x14ac:dyDescent="0.25">
+      <c r="B76" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C76" s="9">
+        <v>1.7700000000000001E-3</v>
+      </c>
+      <c r="D76" s="9">
+        <v>1.2600000000000001E-3</v>
+      </c>
+      <c r="E76" s="10">
+        <v>4.0400000000000002E-3</v>
+      </c>
+      <c r="G76" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H76" s="15">
+        <v>5.8775799999999997E-4</v>
+      </c>
+      <c r="I76" s="23">
+        <v>6.8402000000000003E-4</v>
+      </c>
+      <c r="K76" s="29"/>
+      <c r="L76" s="29"/>
+      <c r="M76" s="29"/>
+      <c r="N76" s="29"/>
+      <c r="O76" s="29"/>
+      <c r="P76" s="29"/>
+      <c r="Q76" s="29"/>
+      <c r="R76" s="29"/>
+      <c r="S76" s="29"/>
+    </row>
+    <row r="77" spans="2:20" ht="24" x14ac:dyDescent="0.25">
+      <c r="B77" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C77" s="9">
+        <v>0.99888999999999994</v>
+      </c>
+      <c r="D77" s="9">
+        <v>0.99955000000000005</v>
+      </c>
+      <c r="E77" s="10">
+        <v>0.99919999999999998</v>
+      </c>
+      <c r="G77" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H77" s="9">
+        <v>0.99973000000000001</v>
+      </c>
+      <c r="I77" s="10">
+        <v>0.99978999999999996</v>
+      </c>
+      <c r="K77" s="31">
+        <f>K74*1000000000000</f>
+        <v>67.391899999999993</v>
+      </c>
+      <c r="L77" s="31">
+        <f t="shared" ref="L77:T78" si="31">L74*1000000000000</f>
+        <v>6.3372999999999999</v>
+      </c>
+      <c r="M77" s="31">
+        <f t="shared" si="31"/>
+        <v>63.460899999999995</v>
+      </c>
+      <c r="N77" s="31">
+        <f t="shared" si="31"/>
+        <v>2.83291</v>
+      </c>
+      <c r="O77" s="31">
+        <f t="shared" si="31"/>
+        <v>29.477299999999996</v>
+      </c>
+      <c r="P77" s="31">
+        <f t="shared" si="31"/>
+        <v>1.6772899999999999</v>
+      </c>
+      <c r="Q77" s="31">
+        <f t="shared" si="31"/>
+        <v>22.883500000000002</v>
+      </c>
+      <c r="R77" s="31">
+        <f t="shared" si="31"/>
+        <v>0.901119</v>
+      </c>
+      <c r="S77" s="31">
+        <f t="shared" si="31"/>
+        <v>10.5525</v>
+      </c>
+      <c r="T77" s="31">
+        <f t="shared" si="31"/>
+        <v>0.80733500000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="2:20" ht="24" x14ac:dyDescent="0.25">
+      <c r="B78" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C78" s="12">
+        <v>0.99856999999999996</v>
+      </c>
+      <c r="D78" s="12">
+        <v>0.99941999999999998</v>
+      </c>
+      <c r="E78" s="13">
+        <v>0.99897999999999998</v>
+      </c>
+      <c r="G78" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H78" s="12">
+        <v>0.99965000000000004</v>
+      </c>
+      <c r="I78" s="13">
+        <v>0.99973000000000001</v>
+      </c>
+      <c r="K78" s="31">
+        <f>K75*1000000000000</f>
+        <v>-36.142800000000001</v>
+      </c>
+      <c r="L78" s="31">
+        <f t="shared" si="31"/>
+        <v>8.9411000000000005</v>
+      </c>
+      <c r="M78" s="31">
+        <f t="shared" si="31"/>
+        <v>-54.948099999999997</v>
+      </c>
+      <c r="N78" s="31">
+        <f t="shared" si="31"/>
+        <v>3.8618999999999999</v>
+      </c>
+      <c r="O78" s="31">
+        <f t="shared" si="31"/>
+        <v>-26.0703</v>
+      </c>
+      <c r="P78" s="31">
+        <f t="shared" si="31"/>
+        <v>2.4865899999999996</v>
+      </c>
+      <c r="Q78" s="31">
+        <f t="shared" si="31"/>
+        <v>-20.799800000000001</v>
+      </c>
+      <c r="R78" s="31">
+        <f t="shared" si="31"/>
+        <v>1.39314</v>
+      </c>
+      <c r="S78" s="31">
+        <f t="shared" si="31"/>
+        <v>-14.3552</v>
+      </c>
+      <c r="T78" s="31">
+        <f t="shared" si="31"/>
+        <v>1.2215099999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="11:26" x14ac:dyDescent="0.25">
+      <c r="S82" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="T82" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="83" spans="11:26" x14ac:dyDescent="0.25">
+      <c r="K83" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L83" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M83" t="s">
+        <v>28</v>
+      </c>
+      <c r="N83" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O83" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S83" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="T83" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="84" spans="11:26" ht="24" x14ac:dyDescent="0.25">
+      <c r="K84" s="3">
+        <v>8000</v>
+      </c>
+      <c r="L84" s="3">
+        <f xml:space="preserve"> K73*100</f>
+        <v>160.012</v>
+      </c>
+      <c r="M84" s="3">
+        <f>L84/$M$1</f>
+        <v>2.0127295597484278</v>
+      </c>
+      <c r="N84" s="3">
+        <f>LN(M84)</f>
+        <v>0.6994917907611814</v>
+      </c>
+      <c r="O84">
+        <f>$M$1/K84</f>
+        <v>9.9375000000000002E-3</v>
+      </c>
+      <c r="P84">
+        <f>O84*1000</f>
+        <v>9.9375</v>
+      </c>
+      <c r="S84" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="T84" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="U84" t="s">
+        <v>35</v>
+      </c>
+      <c r="V84">
+        <v>2.0931099999999998</v>
+      </c>
+      <c r="W84" t="s">
+        <v>19</v>
+      </c>
+      <c r="X84">
+        <f>EXP(V84)</f>
+        <v>8.1100983900842483</v>
+      </c>
+    </row>
+    <row r="85" spans="11:26" ht="24" x14ac:dyDescent="0.25">
+      <c r="K85" s="3">
+        <v>9000</v>
+      </c>
+      <c r="L85" s="3">
+        <f>M73*100</f>
+        <v>169.12899999999999</v>
+      </c>
+      <c r="M85" s="3">
+        <f t="shared" ref="M85:M88" si="32">L85/$M$1</f>
+        <v>2.1274088050314464</v>
+      </c>
+      <c r="N85" s="3">
+        <f t="shared" ref="N85:N88" si="33">LN(M85)</f>
+        <v>0.75490471569658424</v>
+      </c>
+      <c r="O85">
+        <f t="shared" ref="O85:O88" si="34">$M$1/K85</f>
+        <v>8.8333333333333337E-3</v>
+      </c>
+      <c r="P85">
+        <f t="shared" ref="P85:P88" si="35">O85*1000</f>
+        <v>8.8333333333333339</v>
+      </c>
+      <c r="S85" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="T85" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="U85" t="s">
+        <v>37</v>
+      </c>
+      <c r="V85">
+        <v>0.15720000000000001</v>
+      </c>
+      <c r="W85" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X85">
+        <f t="shared" ref="X85:X87" si="36">EXP(V85)</f>
+        <v>1.1702296364251661</v>
+      </c>
+      <c r="Y85" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z85">
+        <f>X85/X84</f>
+        <v>0.14429290251964622</v>
+      </c>
+    </row>
+    <row r="86" spans="11:26" ht="24" x14ac:dyDescent="0.25">
+      <c r="K86" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L86" s="3">
+        <f>O73*100</f>
+        <v>203.33500000000001</v>
+      </c>
+      <c r="M86" s="3">
+        <f t="shared" si="32"/>
+        <v>2.557672955974843</v>
+      </c>
+      <c r="N86" s="3">
+        <f t="shared" si="33"/>
+        <v>0.93909784352667969</v>
+      </c>
+      <c r="O86">
+        <f t="shared" si="34"/>
+        <v>7.9500000000000005E-3</v>
+      </c>
+      <c r="P86">
+        <f t="shared" si="35"/>
+        <v>7.95</v>
+      </c>
+      <c r="S86" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="T86" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="U86" t="s">
+        <v>36</v>
+      </c>
+      <c r="V86">
+        <v>-0.14474999999999999</v>
+      </c>
+      <c r="W86" t="s">
+        <v>20</v>
+      </c>
+      <c r="X86">
+        <f>V86*-1*1000</f>
+        <v>144.75</v>
+      </c>
+    </row>
+    <row r="87" spans="11:26" ht="24" x14ac:dyDescent="0.25">
+      <c r="K87" s="3">
+        <v>11000</v>
+      </c>
+      <c r="L87" s="3">
+        <f>Q73*100</f>
+        <v>221.67099999999999</v>
+      </c>
+      <c r="M87" s="3">
+        <f t="shared" si="32"/>
+        <v>2.788314465408805</v>
+      </c>
+      <c r="N87" s="3">
+        <f t="shared" si="33"/>
+        <v>1.025437279008562</v>
+      </c>
+      <c r="O87">
+        <f t="shared" si="34"/>
+        <v>7.2272727272727271E-3</v>
+      </c>
+      <c r="P87">
+        <f t="shared" si="35"/>
+        <v>7.2272727272727275</v>
+      </c>
+      <c r="S87" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="T87" s="10">
+        <v>7.5799999999999999E-3</v>
+      </c>
+      <c r="U87" t="s">
+        <v>37</v>
+      </c>
+      <c r="V87">
+        <v>1.917E-2</v>
+      </c>
+      <c r="W87" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X87">
+        <f t="shared" si="36"/>
+        <v>1.0193549242256823</v>
+      </c>
+      <c r="Y87" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z87">
+        <f>X87/X86</f>
+        <v>7.042175642319049E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="11:26" x14ac:dyDescent="0.25">
+      <c r="K88" s="3">
+        <v>12000</v>
+      </c>
+      <c r="L88" s="3">
+        <f>S73*100</f>
+        <v>257.03699999999998</v>
+      </c>
+      <c r="M88" s="3">
+        <f t="shared" si="32"/>
+        <v>3.2331698113207543</v>
+      </c>
+      <c r="N88" s="3">
+        <f t="shared" si="33"/>
+        <v>1.1734630217440054</v>
+      </c>
+      <c r="O88">
+        <f t="shared" si="34"/>
+        <v>6.6249999999999998E-3</v>
+      </c>
+      <c r="P88">
+        <f t="shared" si="35"/>
+        <v>6.625</v>
+      </c>
+      <c r="S88" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="T88" s="10">
+        <v>-0.97467999999999999</v>
+      </c>
+      <c r="W88" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X88">
+        <f>X86/X84</f>
+        <v>17.848118855990393</v>
+      </c>
+    </row>
+    <row r="89" spans="11:26" ht="24" x14ac:dyDescent="0.25">
+      <c r="S89" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="T89" s="10">
+        <v>0.95</v>
+      </c>
+      <c r="W89" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X89">
+        <f>X88*Z89</f>
+        <v>2.578422173001786</v>
+      </c>
+      <c r="Y89" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z89">
+        <f>SQRT((Z85^2)+(Z87^2))</f>
+        <v>0.14446464603951167</v>
+      </c>
+    </row>
+    <row r="90" spans="11:26" x14ac:dyDescent="0.25">
+      <c r="S90" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="T90" s="13">
+        <v>0.93332999999999999</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="N43:P43"/>
-    <mergeCell ref="N44:P44"/>
+  <mergeCells count="6">
+    <mergeCell ref="Q43:T43"/>
+    <mergeCell ref="Q44:T44"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="H71:I71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
01: Correction with iposun
</commit_message>
<xml_diff>
--- a/01_Townsend/data/Townsend.xlsx
+++ b/01_Townsend/data/Townsend.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\Škola Mgr\Praktikum plazma\PraktikaPlazma\01_Townsend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D0A2E6-ECBD-4438-A2EC-F7C477A16C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD1F61E-F3B3-4880-8145-2188DA68F44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27555" yWindow="3030" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -573,24 +573,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="11" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -612,6 +594,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -952,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G70" workbookViewId="0">
-      <selection activeCell="X90" sqref="X90"/>
+    <sheetView tabSelected="1" topLeftCell="O64" workbookViewId="0">
+      <selection activeCell="X88" sqref="X88:X89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3250,11 +3250,11 @@
         <v>-20.505201831375501</v>
       </c>
       <c r="O43" s="7"/>
-      <c r="P43" s="24"/>
-      <c r="Q43" s="17"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
-      <c r="T43" s="19"/>
+      <c r="P43" s="18"/>
+      <c r="Q43" s="26"/>
+      <c r="R43" s="27"/>
+      <c r="S43" s="27"/>
+      <c r="T43" s="28"/>
     </row>
     <row r="44" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44">
@@ -3298,11 +3298,11 @@
         <v>-20.964488501660526</v>
       </c>
       <c r="O44" s="8"/>
-      <c r="P44" s="25"/>
-      <c r="Q44" s="20"/>
-      <c r="R44" s="21"/>
-      <c r="S44" s="21"/>
-      <c r="T44" s="22"/>
+      <c r="P44" s="19"/>
+      <c r="Q44" s="29"/>
+      <c r="R44" s="30"/>
+      <c r="S44" s="30"/>
+      <c r="T44" s="31"/>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45">
@@ -3346,7 +3346,7 @@
         <v>-21.461410383437091</v>
       </c>
       <c r="O45" s="8"/>
-      <c r="P45" s="26"/>
+      <c r="P45" s="20"/>
       <c r="Q45" s="9"/>
       <c r="R45" s="9"/>
       <c r="S45" s="9"/>
@@ -3394,7 +3394,7 @@
         <v>-21.920594098553678</v>
       </c>
       <c r="O46" s="8"/>
-      <c r="P46" s="26"/>
+      <c r="P46" s="20"/>
       <c r="Q46" s="9"/>
       <c r="R46" s="9"/>
       <c r="S46" s="9"/>
@@ -3443,7 +3443,7 @@
         <v>-22.432524084662724</v>
       </c>
       <c r="O47" s="8"/>
-      <c r="P47" s="26"/>
+      <c r="P47" s="20"/>
       <c r="Q47" s="9"/>
       <c r="R47" s="9"/>
       <c r="S47" s="9"/>
@@ -3492,7 +3492,7 @@
         <v>-22.877430924822182</v>
       </c>
       <c r="O48" s="8"/>
-      <c r="P48" s="26"/>
+      <c r="P48" s="20"/>
       <c r="Q48" s="9"/>
       <c r="R48" s="9"/>
       <c r="S48" s="9"/>
@@ -3541,7 +3541,7 @@
         <v>-23.431316038048621</v>
       </c>
       <c r="O49" s="8"/>
-      <c r="P49" s="26"/>
+      <c r="P49" s="20"/>
       <c r="Q49" s="9"/>
       <c r="R49" s="9"/>
       <c r="S49" s="15"/>
@@ -3589,7 +3589,7 @@
         <v>-24.056804570134751</v>
       </c>
       <c r="O50" s="8"/>
-      <c r="P50" s="26"/>
+      <c r="P50" s="20"/>
       <c r="Q50" s="9"/>
       <c r="R50" s="9"/>
       <c r="S50" s="9"/>
@@ -3637,7 +3637,7 @@
         <v>-24.945443770678398</v>
       </c>
       <c r="O51" s="11"/>
-      <c r="P51" s="27"/>
+      <c r="P51" s="21"/>
       <c r="Q51" s="12"/>
       <c r="R51" s="12"/>
       <c r="S51" s="12"/>
@@ -3660,7 +3660,7 @@
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
       <c r="Q53" s="7"/>
-      <c r="R53" s="24"/>
+      <c r="R53" s="18"/>
       <c r="S53" s="14"/>
       <c r="T53" s="7"/>
       <c r="U53" s="14"/>
@@ -3683,7 +3683,7 @@
         <v>3</v>
       </c>
       <c r="Q54" s="8"/>
-      <c r="R54" s="25"/>
+      <c r="R54" s="19"/>
       <c r="S54" s="10"/>
       <c r="T54" s="8"/>
       <c r="U54" s="10"/>
@@ -3731,7 +3731,7 @@
         <v>-20.101435655137511</v>
       </c>
       <c r="Q55" s="8"/>
-      <c r="R55" s="25"/>
+      <c r="R55" s="19"/>
       <c r="S55" s="10"/>
       <c r="T55" s="8"/>
       <c r="U55" s="10"/>
@@ -3779,7 +3779,7 @@
         <v>-20.68052568327025</v>
       </c>
       <c r="Q56" s="8"/>
-      <c r="R56" s="25"/>
+      <c r="R56" s="19"/>
       <c r="S56" s="10"/>
       <c r="T56" s="8"/>
       <c r="U56" s="10"/>
@@ -3826,7 +3826,7 @@
         <v>-21.236316155734514</v>
       </c>
       <c r="Q57" s="8"/>
-      <c r="R57" s="25"/>
+      <c r="R57" s="19"/>
       <c r="S57" s="10"/>
       <c r="T57" s="8"/>
       <c r="U57" s="10"/>
@@ -3873,7 +3873,7 @@
         <v>-21.762666265982674</v>
       </c>
       <c r="Q58" s="8"/>
-      <c r="R58" s="25"/>
+      <c r="R58" s="19"/>
       <c r="S58" s="10"/>
       <c r="T58" s="8"/>
       <c r="U58" s="10"/>
@@ -3920,7 +3920,7 @@
         <v>-22.216403293684351</v>
       </c>
       <c r="Q59" s="8"/>
-      <c r="R59" s="25"/>
+      <c r="R59" s="19"/>
       <c r="S59" s="10"/>
       <c r="T59" s="8"/>
       <c r="U59" s="10"/>
@@ -3967,7 +3967,7 @@
         <v>-22.802707378626248</v>
       </c>
       <c r="Q60" s="8"/>
-      <c r="R60" s="25"/>
+      <c r="R60" s="19"/>
       <c r="S60" s="10"/>
       <c r="T60" s="8"/>
       <c r="U60" s="10"/>
@@ -4014,7 +4014,7 @@
         <v>-23.295911401042417</v>
       </c>
       <c r="Q61" s="11"/>
-      <c r="R61" s="28"/>
+      <c r="R61" s="22"/>
       <c r="S61" s="13"/>
       <c r="T61" s="11"/>
       <c r="U61" s="13"/>
@@ -4154,35 +4154,35 @@
       <c r="B70" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C70" s="17" t="s">
+      <c r="C70" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D70" s="18"/>
-      <c r="E70" s="19"/>
+      <c r="D70" s="27"/>
+      <c r="E70" s="28"/>
       <c r="G70" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H70" s="17" t="s">
+      <c r="H70" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="I70" s="19"/>
+      <c r="I70" s="28"/>
     </row>
     <row r="71" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B71" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C71" s="20" t="s">
+      <c r="C71" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="D71" s="21"/>
-      <c r="E71" s="22"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="31"/>
       <c r="G71" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H71" s="20" t="s">
+      <c r="H71" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="I71" s="22"/>
+      <c r="I71" s="31"/>
     </row>
     <row r="72" spans="2:20" ht="24" x14ac:dyDescent="0.25">
       <c r="B72" s="8" t="s">
@@ -4206,34 +4206,34 @@
       <c r="I72" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="K72" s="29">
+      <c r="K72" s="23">
         <v>80</v>
       </c>
-      <c r="L72" s="29" t="s">
+      <c r="L72" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="M72" s="29">
+      <c r="M72" s="23">
         <v>90</v>
       </c>
-      <c r="N72" s="29" t="s">
+      <c r="N72" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="O72" s="29">
+      <c r="O72" s="23">
         <v>100</v>
       </c>
-      <c r="P72" s="29" t="s">
+      <c r="P72" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="Q72" s="30">
+      <c r="Q72" s="24">
         <v>110</v>
       </c>
-      <c r="R72" s="29" t="s">
+      <c r="R72" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="S72" s="30">
+      <c r="S72" s="24">
         <v>120</v>
       </c>
-      <c r="T72" s="29" t="s">
+      <c r="T72" s="23" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4318,34 +4318,34 @@
       <c r="J74" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K74" s="29">
+      <c r="K74" s="23">
         <v>6.7391899999999998E-11</v>
       </c>
-      <c r="L74" s="29">
+      <c r="L74" s="23">
         <v>6.3372999999999997E-12</v>
       </c>
-      <c r="M74" s="29">
+      <c r="M74" s="23">
         <v>6.3460899999999996E-11</v>
       </c>
-      <c r="N74" s="29">
+      <c r="N74" s="23">
         <v>2.8329099999999999E-12</v>
       </c>
-      <c r="O74" s="29">
+      <c r="O74" s="23">
         <v>2.9477299999999997E-11</v>
       </c>
-      <c r="P74" s="29">
+      <c r="P74" s="23">
         <v>1.67729E-12</v>
       </c>
-      <c r="Q74" s="29">
+      <c r="Q74" s="23">
         <v>2.28835E-11</v>
       </c>
-      <c r="R74" s="29">
+      <c r="R74" s="23">
         <v>9.0111900000000003E-13</v>
       </c>
-      <c r="S74" s="29">
+      <c r="S74" s="23">
         <v>1.0552500000000001E-11</v>
       </c>
-      <c r="T74" s="29">
+      <c r="T74" s="23">
         <v>8.0733500000000001E-13</v>
       </c>
     </row>
@@ -4374,34 +4374,34 @@
       <c r="J75" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="K75" s="29">
+      <c r="K75" s="23">
         <v>-3.6142799999999998E-11</v>
       </c>
-      <c r="L75" s="29">
+      <c r="L75" s="23">
         <v>8.9411000000000003E-12</v>
       </c>
-      <c r="M75" s="29">
+      <c r="M75" s="23">
         <v>-5.4948099999999997E-11</v>
       </c>
-      <c r="N75" s="29">
+      <c r="N75" s="23">
         <v>3.8618999999999999E-12</v>
       </c>
-      <c r="O75" s="29">
+      <c r="O75" s="23">
         <v>-2.6070299999999999E-11</v>
       </c>
-      <c r="P75" s="29">
+      <c r="P75" s="23">
         <v>2.4865899999999998E-12</v>
       </c>
-      <c r="Q75" s="29">
+      <c r="Q75" s="23">
         <v>-2.0799799999999999E-11</v>
       </c>
-      <c r="R75" s="29">
+      <c r="R75" s="23">
         <v>1.3931400000000001E-12</v>
       </c>
-      <c r="S75" s="29">
+      <c r="S75" s="23">
         <v>-1.4355199999999999E-11</v>
       </c>
-      <c r="T75" s="29">
+      <c r="T75" s="23">
         <v>1.2215099999999999E-12</v>
       </c>
     </row>
@@ -4424,18 +4424,18 @@
       <c r="H76" s="15">
         <v>5.8775799999999997E-4</v>
       </c>
-      <c r="I76" s="23">
+      <c r="I76" s="17">
         <v>6.8402000000000003E-4</v>
       </c>
-      <c r="K76" s="29"/>
-      <c r="L76" s="29"/>
-      <c r="M76" s="29"/>
-      <c r="N76" s="29"/>
-      <c r="O76" s="29"/>
-      <c r="P76" s="29"/>
-      <c r="Q76" s="29"/>
-      <c r="R76" s="29"/>
-      <c r="S76" s="29"/>
+      <c r="K76" s="23"/>
+      <c r="L76" s="23"/>
+      <c r="M76" s="23"/>
+      <c r="N76" s="23"/>
+      <c r="O76" s="23"/>
+      <c r="P76" s="23"/>
+      <c r="Q76" s="23"/>
+      <c r="R76" s="23"/>
+      <c r="S76" s="23"/>
     </row>
     <row r="77" spans="2:20" ht="24" x14ac:dyDescent="0.25">
       <c r="B77" s="8" t="s">
@@ -4459,43 +4459,43 @@
       <c r="I77" s="10">
         <v>0.99978999999999996</v>
       </c>
-      <c r="K77" s="31">
+      <c r="K77" s="25">
         <f>K74*1000000000000</f>
         <v>67.391899999999993</v>
       </c>
-      <c r="L77" s="31">
+      <c r="L77" s="25">
         <f t="shared" ref="L77:T78" si="31">L74*1000000000000</f>
         <v>6.3372999999999999</v>
       </c>
-      <c r="M77" s="31">
+      <c r="M77" s="25">
         <f t="shared" si="31"/>
         <v>63.460899999999995</v>
       </c>
-      <c r="N77" s="31">
+      <c r="N77" s="25">
         <f t="shared" si="31"/>
         <v>2.83291</v>
       </c>
-      <c r="O77" s="31">
+      <c r="O77" s="25">
         <f t="shared" si="31"/>
         <v>29.477299999999996</v>
       </c>
-      <c r="P77" s="31">
+      <c r="P77" s="25">
         <f t="shared" si="31"/>
         <v>1.6772899999999999</v>
       </c>
-      <c r="Q77" s="31">
+      <c r="Q77" s="25">
         <f t="shared" si="31"/>
         <v>22.883500000000002</v>
       </c>
-      <c r="R77" s="31">
+      <c r="R77" s="25">
         <f t="shared" si="31"/>
         <v>0.901119</v>
       </c>
-      <c r="S77" s="31">
+      <c r="S77" s="25">
         <f t="shared" si="31"/>
         <v>10.5525</v>
       </c>
-      <c r="T77" s="31">
+      <c r="T77" s="25">
         <f t="shared" si="31"/>
         <v>0.80733500000000002</v>
       </c>
@@ -4522,43 +4522,43 @@
       <c r="I78" s="13">
         <v>0.99973000000000001</v>
       </c>
-      <c r="K78" s="31">
+      <c r="K78" s="25">
         <f>K75*1000000000000</f>
         <v>-36.142800000000001</v>
       </c>
-      <c r="L78" s="31">
+      <c r="L78" s="25">
         <f t="shared" si="31"/>
         <v>8.9411000000000005</v>
       </c>
-      <c r="M78" s="31">
+      <c r="M78" s="25">
         <f t="shared" si="31"/>
         <v>-54.948099999999997</v>
       </c>
-      <c r="N78" s="31">
+      <c r="N78" s="25">
         <f t="shared" si="31"/>
         <v>3.8618999999999999</v>
       </c>
-      <c r="O78" s="31">
+      <c r="O78" s="25">
         <f t="shared" si="31"/>
         <v>-26.0703</v>
       </c>
-      <c r="P78" s="31">
+      <c r="P78" s="25">
         <f t="shared" si="31"/>
         <v>2.4865899999999996</v>
       </c>
-      <c r="Q78" s="31">
+      <c r="Q78" s="25">
         <f t="shared" si="31"/>
         <v>-20.799800000000001</v>
       </c>
-      <c r="R78" s="31">
+      <c r="R78" s="25">
         <f t="shared" si="31"/>
         <v>1.39314</v>
       </c>
-      <c r="S78" s="31">
+      <c r="S78" s="25">
         <f t="shared" si="31"/>
         <v>-14.3552</v>
       </c>
-      <c r="T78" s="31">
+      <c r="T78" s="25">
         <f t="shared" si="31"/>
         <v>1.2215099999999999</v>
       </c>
@@ -4633,7 +4633,7 @@
       <c r="W84" t="s">
         <v>19</v>
       </c>
-      <c r="X84">
+      <c r="X84" s="25">
         <f>EXP(V84)</f>
         <v>8.1100983900842483</v>
       </c>
@@ -4677,7 +4677,7 @@
       <c r="W85" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="X85">
+      <c r="X85" s="25">
         <f t="shared" ref="X85:X87" si="36">EXP(V85)</f>
         <v>1.1702296364251661</v>
       </c>
@@ -4728,7 +4728,7 @@
       <c r="W86" t="s">
         <v>20</v>
       </c>
-      <c r="X86">
+      <c r="X86" s="25">
         <f>V86*-1*1000</f>
         <v>144.75</v>
       </c>
@@ -4772,7 +4772,7 @@
       <c r="W87" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="X87">
+      <c r="X87" s="25">
         <f t="shared" si="36"/>
         <v>1.0193549242256823</v>
       </c>
@@ -4817,7 +4817,7 @@
       <c r="W88" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X88">
+      <c r="X88" s="25">
         <f>X86/X84</f>
         <v>17.848118855990393</v>
       </c>
@@ -4832,7 +4832,7 @@
       <c r="W89" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="X89">
+      <c r="X89" s="25">
         <f>X88*Z89</f>
         <v>2.578422173001786</v>
       </c>

</xml_diff>